<commit_message>
Updated CHE model - 2025-07-31 15:33
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE/ReportDefs_vervestacks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D3B86D-5E44-469A-9BFD-27A22346152F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AD581D-C637-43E8-9A19-5097D8EA4F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="145">
   <si>
     <t>Unit</t>
   </si>
@@ -115,9 +115,6 @@
     <t>TS</t>
   </si>
   <si>
-    <t>ELC</t>
-  </si>
-  <si>
     <t>VAR_CAP</t>
   </si>
   <si>
@@ -391,9 +388,6 @@
     <t>c_neg_andor</t>
   </si>
   <si>
-    <t>ELE,STG</t>
-  </si>
-  <si>
     <t>Elec New Capacity</t>
   </si>
   <si>
@@ -472,9 +466,6 @@
     <t>Wind</t>
   </si>
   <si>
-    <t>-ElcAgg*</t>
-  </si>
-  <si>
     <t>p,t</t>
   </si>
   <si>
@@ -506,6 +497,24 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>Trd*</t>
+  </si>
+  <si>
+    <t>Trade</t>
+  </si>
+  <si>
+    <t>ELE,STG,IRE</t>
+  </si>
+  <si>
+    <t>ELE,IRE</t>
+  </si>
+  <si>
+    <t>-ElcAgg*,-*EV*</t>
+  </si>
+  <si>
+    <t>ELC,ELC_???-???</t>
   </si>
 </sst>
 </file>
@@ -1069,55 +1078,55 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="B1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" t="s">
-        <v>48</v>
-      </c>
       <c r="L1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
       </c>
       <c r="N1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="I2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
         <v>49</v>
-      </c>
-      <c r="L2" t="s">
-        <v>50</v>
       </c>
       <c r="M2" t="s">
         <v>6</v>
       </c>
       <c r="N2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" t="s">
         <v>86</v>
-      </c>
-      <c r="H4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1126,10 +1135,10 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5" t="str">
         <f>"sg_"&amp;I2</f>
@@ -1174,7 +1183,7 @@
         <v>Fixed</v>
       </c>
       <c r="I6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -1202,7 +1211,7 @@
         <v>V1G</v>
       </c>
       <c r="I7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O7">
         <v>2</v>
@@ -1230,7 +1239,7 @@
         <v>V2G</v>
       </c>
       <c r="I8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O8">
         <v>3</v>
@@ -1256,18 +1265,18 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -1276,10 +1285,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
         <v>56</v>
-      </c>
-      <c r="G2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1314,32 +1323,32 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <f>1/8.76</f>
@@ -1348,13 +1357,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D4">
         <f>1/8.76*100</f>
@@ -1371,9 +1380,9 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -1404,39 +1413,39 @@
   <sheetData>
     <row r="1" spans="1:21" ht="17.25" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15" thickTop="1" thickBot="1">
       <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>0</v>
@@ -1445,7 +1454,7 @@
         <v>10</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>2</v>
@@ -1454,56 +1463,62 @@
         <v>1</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K3" t="s">
-        <v>13</v>
-      </c>
       <c r="N3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" t="s">
+        <v>102</v>
+      </c>
+      <c r="P4" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" t="s">
-        <v>104</v>
-      </c>
-      <c r="P4" t="s">
-        <v>46</v>
-      </c>
       <c r="Q4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U4" s="8"/>
     </row>
@@ -1511,125 +1526,134 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>142</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="I5" t="s">
-        <v>11</v>
+        <v>144</v>
       </c>
       <c r="K5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="P5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K6" t="s">
+        <v>109</v>
+      </c>
+      <c r="N6" t="s">
+        <v>57</v>
+      </c>
+      <c r="P6" t="s">
         <v>78</v>
       </c>
-      <c r="C6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="K6" t="s">
-        <v>111</v>
-      </c>
-      <c r="N6" t="s">
-        <v>58</v>
-      </c>
-      <c r="P6" t="s">
-        <v>79</v>
-      </c>
       <c r="Q6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K7" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" t="s">
+        <v>105</v>
+      </c>
+      <c r="P7" t="s">
         <v>38</v>
-      </c>
-      <c r="K7" t="s">
-        <v>59</v>
-      </c>
-      <c r="N7" t="s">
-        <v>107</v>
-      </c>
-      <c r="P7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="N8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P8" t="s">
         <v>62</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>63</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
+        <v>107</v>
+      </c>
+      <c r="N9" t="s">
         <v>65</v>
       </c>
-      <c r="K9" t="s">
-        <v>109</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q9" t="s">
         <v>66</v>
-      </c>
-      <c r="P9" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="N10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1645,7 +1669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A8EC7F-95E3-4526-8B78-C58A96098159}">
   <dimension ref="C1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -1664,15 +1688,15 @@
   <sheetData>
     <row r="1" spans="3:11">
       <c r="C1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="3:11">
       <c r="C2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -1681,42 +1705,42 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="3:11">
       <c r="C3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1744,18 +1768,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1779,18 +1803,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1818,18 +1842,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1854,18 +1878,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>72</v>
-      </c>
-      <c r="C2" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1875,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10ADB714-E6AA-4E3E-B77B-62B65BA0E218}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1893,71 +1917,71 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
       <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
         <v>89</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>90</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>91</v>
-      </c>
-      <c r="G2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" t="str">
         <f>D3</f>
         <v>CCGT</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ref="C4:C20" si="0">D4</f>
         <v>Int Comb</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
         <v>Gas_Oil Steam</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -1969,67 +1993,67 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>OCGT (Peaker)</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>Subcritical Coal</v>
       </c>
       <c r="D8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>Supercritical Coal</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>IGCC</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>Bioenergy</v>
       </c>
       <c r="D11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -2041,43 +2065,43 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>Wind onshore</v>
       </c>
       <c r="D13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>Wind offshore</v>
       </c>
       <c r="D14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>Geothermal</v>
       </c>
       <c r="D15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -2089,7 +2113,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -2101,46 +2125,46 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>Hydro pumped stg</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>Util Batt Stg</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>EV Batt</v>
       </c>
       <c r="D20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -2148,13 +2172,24 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C22" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2182,33 +2217,33 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
       <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
         <v>98</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
         <v>99</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>101</v>
-      </c>
-      <c r="G2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H2" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CHE model - 2025-08-15 15:09
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE/ReportDefs_vervestacks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE8D2E2-3532-4203-B088-884C639FA604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5084DB-70AB-4280-8176-3DF29E338507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="169">
   <si>
     <t>Unit</t>
   </si>
@@ -584,6 +584,9 @@
   </si>
   <si>
     <t>$/tCO2</t>
+  </si>
+  <si>
+    <t>ELE,STG,IRE,-Grid</t>
   </si>
 </sst>
 </file>
@@ -1829,7 +1832,7 @@
   <sheetPr codeName="Sheet31"/>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1947,9 +1950,9 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -1965,11 +1968,11 @@
     <col min="10" max="10" width="8.59765625" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="8.73046875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.73046875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="38.265625" customWidth="1"/>
-    <col min="17" max="17" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.53125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.59765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.53125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="2.1328125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.86328125" bestFit="1" customWidth="1"/>
@@ -2108,7 +2111,11 @@
         <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>168</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="H6" t="s">
+        <v>28</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
Updated CHE model - 2025-08-16 12:05
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE/ReportDefs_vervestacks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5084DB-70AB-4280-8176-3DF29E338507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B09016-70C2-4AF1-A252-6411BA1F4B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="PSet_MAP coarse" sheetId="57" r:id="rId4"/>
     <sheet name="CSET_MAP" sheetId="66" r:id="rId5"/>
     <sheet name="CName_MAP" sheetId="58" r:id="rId6"/>
-    <sheet name="varbl map" sheetId="64" r:id="rId7"/>
+    <sheet name="timeslice map" sheetId="64" r:id="rId7"/>
     <sheet name="process map" sheetId="65" r:id="rId8"/>
     <sheet name="commodity map" sheetId="67" r:id="rId9"/>
     <sheet name="ATS" sheetId="63" r:id="rId10"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="181">
   <si>
     <t>Unit</t>
   </si>
@@ -250,9 +250,6 @@
     <t>process</t>
   </si>
   <si>
-    <t>~Varbl_map</t>
-  </si>
-  <si>
     <t>dimension</t>
   </si>
   <si>
@@ -587,6 +584,45 @@
   </si>
   <si>
     <t>ELE,STG,IRE,-Grid</t>
+  </si>
+  <si>
+    <t>s?a*</t>
+  </si>
+  <si>
+    <t>*,-s?a*</t>
+  </si>
+  <si>
+    <t>hourly</t>
+  </si>
+  <si>
+    <t>aggregated</t>
+  </si>
+  <si>
+    <t>ts_type</t>
+  </si>
+  <si>
+    <t>ts_season</t>
+  </si>
+  <si>
+    <t>S1*</t>
+  </si>
+  <si>
+    <t>S2*</t>
+  </si>
+  <si>
+    <t>S3*</t>
+  </si>
+  <si>
+    <t>S4*</t>
+  </si>
+  <si>
+    <t>S5*</t>
+  </si>
+  <si>
+    <t>S6*</t>
+  </si>
+  <si>
+    <t>~Timeslice_Map</t>
   </si>
 </sst>
 </file>
@@ -1146,13 +1182,13 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" t="s">
         <v>131</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>132</v>
-      </c>
-      <c r="C1" t="s">
-        <v>133</v>
       </c>
       <c r="H1" t="s">
         <v>39</v>
@@ -1160,18 +1196,18 @@
     </row>
     <row r="2" spans="1:16">
       <c r="H2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" t="s">
         <v>134</v>
-      </c>
-      <c r="I2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
         <v>66</v>
-      </c>
-      <c r="G4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1213,16 +1249,16 @@
         <v>Delayed transition_3d</v>
       </c>
       <c r="H6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1239,16 +1275,16 @@
         <v>Net Zero 2050_3d</v>
       </c>
       <c r="H7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N7">
         <v>2</v>
       </c>
       <c r="P7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1265,16 +1301,16 @@
         <v>NDCs_3d</v>
       </c>
       <c r="H8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N8">
         <v>3</v>
       </c>
       <c r="P8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1291,16 +1327,16 @@
         <v>Below 2deg_3d</v>
       </c>
       <c r="H9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I9" t="s">
         <v>142</v>
-      </c>
-      <c r="I9" t="s">
-        <v>143</v>
       </c>
       <c r="N9">
         <v>4</v>
       </c>
       <c r="P9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1317,16 +1353,16 @@
         <v>Current Policies_3d</v>
       </c>
       <c r="H10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N10">
         <v>5</v>
       </c>
       <c r="P10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1343,16 +1379,16 @@
         <v>Low demand_3d</v>
       </c>
       <c r="H11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N11">
         <v>6</v>
       </c>
       <c r="P11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1369,16 +1405,16 @@
         <v>Fragmented World_3d</v>
       </c>
       <c r="H12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N12">
         <v>7</v>
       </c>
       <c r="P12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1399,14 +1435,14 @@
         <v>Delayed transition</v>
       </c>
       <c r="I13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N13">
         <f>N6</f>
         <v>1</v>
       </c>
       <c r="P13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1427,14 +1463,14 @@
         <v>Net Zero 2050</v>
       </c>
       <c r="I14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N14">
         <f t="shared" ref="N14:N26" si="5">N7</f>
         <v>2</v>
       </c>
       <c r="P14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1455,14 +1491,14 @@
         <v>NDCs</v>
       </c>
       <c r="I15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N15">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1483,14 +1519,14 @@
         <v>Below 2deg</v>
       </c>
       <c r="I16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N16">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1511,14 +1547,14 @@
         <v>Current Policies</v>
       </c>
       <c r="I17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N17">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1539,14 +1575,14 @@
         <v>Low demand</v>
       </c>
       <c r="I18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N18">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1567,14 +1603,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N19">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1595,14 +1631,14 @@
         <v>Delayed transition</v>
       </c>
       <c r="I20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N20">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1623,14 +1659,14 @@
         <v>Net Zero 2050</v>
       </c>
       <c r="I21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N21">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="P21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1651,14 +1687,14 @@
         <v>NDCs</v>
       </c>
       <c r="I22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1679,14 +1715,14 @@
         <v>Below 2deg</v>
       </c>
       <c r="I23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N23">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1707,14 +1743,14 @@
         <v>Current Policies</v>
       </c>
       <c r="I24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N24">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1735,14 +1771,14 @@
         <v>Low demand</v>
       </c>
       <c r="I25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N25">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -1763,14 +1799,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N26">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1870,10 +1906,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="s">
         <v>89</v>
-      </c>
-      <c r="B3" t="s">
-        <v>90</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -1885,13 +1921,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4">
         <f>1/8.76*100</f>
@@ -1900,13 +1936,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D5">
         <v>1E-3</v>
@@ -1914,13 +1950,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D6">
         <v>-1E-3</v>
@@ -1928,13 +1964,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D7">
         <v>-1000</v>
@@ -1950,7 +1986,7 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
@@ -2036,10 +2072,10 @@
         <v>12</v>
       </c>
       <c r="Q2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -2047,16 +2083,16 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K3" t="s">
         <v>10</v>
       </c>
       <c r="N3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -2064,16 +2100,16 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K4" t="s">
         <v>10</v>
       </c>
       <c r="N4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T4" s="8" t="s">
         <v>46</v>
@@ -2085,19 +2121,19 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="I5" t="s">
         <v>123</v>
       </c>
-      <c r="I5" t="s">
-        <v>124</v>
-      </c>
       <c r="K5" t="s">
+        <v>83</v>
+      </c>
+      <c r="N5" t="s">
         <v>84</v>
-      </c>
-      <c r="N5" t="s">
-        <v>85</v>
       </c>
       <c r="T5" s="3" t="s">
         <v>47</v>
@@ -2108,26 +2144,26 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D6" s="2"/>
       <c r="H6" t="s">
         <v>28</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N6" t="s">
         <v>44</v>
       </c>
       <c r="Q6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
@@ -2137,13 +2173,13 @@
         <v>7</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
@@ -2153,13 +2189,13 @@
         <v>7</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
@@ -2169,16 +2205,16 @@
         <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K9" t="s">
         <v>45</v>
       </c>
       <c r="N9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -2186,13 +2222,13 @@
         <v>31</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H10" t="s">
         <v>28</v>
       </c>
       <c r="K10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N10" t="s">
         <v>48</v>
@@ -2209,16 +2245,16 @@
         <v>31</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I11" t="s">
+        <v>163</v>
+      </c>
+      <c r="K11" t="s">
         <v>164</v>
       </c>
-      <c r="K11" t="s">
+      <c r="N11" t="s">
         <v>165</v>
-      </c>
-      <c r="N11" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -2226,7 +2262,7 @@
         <v>51</v>
       </c>
       <c r="K12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N12" t="s">
         <v>52</v>
@@ -2240,16 +2276,16 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>38</v>
       </c>
       <c r="K13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q13" t="s">
         <v>47</v>
@@ -2287,15 +2323,15 @@
   <sheetData>
     <row r="1" spans="3:11">
       <c r="C1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="3:11">
       <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
         <v>110</v>
-      </c>
-      <c r="D2" t="s">
-        <v>111</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -2304,16 +2340,16 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" t="s">
         <v>112</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>113</v>
-      </c>
-      <c r="J2" t="s">
-        <v>114</v>
       </c>
       <c r="K2" t="s">
         <v>12</v>
@@ -2321,22 +2357,22 @@
     </row>
     <row r="3" spans="3:11">
       <c r="C3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" t="s">
         <v>115</v>
-      </c>
-      <c r="F3" t="s">
-        <v>116</v>
       </c>
       <c r="G3" t="s">
         <v>47</v>
       </c>
       <c r="I3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J3" t="s">
         <v>47</v>
@@ -2402,12 +2438,12 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2464,31 +2500,127 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32957E82-8232-40A9-A839-CC5F79005B92}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" t="s">
-        <v>59</v>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" t="str">
+        <f>LEFT(B5,2)</f>
+        <v>S1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" ref="C6:C10" si="0">LEFT(B6,2)</f>
+        <v>S2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>S3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>S4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>S5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>S6</v>
       </c>
     </row>
   </sheetData>
@@ -2516,71 +2648,71 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17.25" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1" thickBot="1">
       <c r="A2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="D2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" t="str">
         <f>D3</f>
         <v>CCGT</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ref="C4:C20" si="0">D4</f>
         <v>Int Comb</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
         <v>Gas_Oil Steam</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -2592,67 +2724,67 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>OCGT (Peaker)</v>
       </c>
       <c r="D7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>Subcritical Coal</v>
       </c>
       <c r="D8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>Supercritical Coal</v>
       </c>
       <c r="D9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>IGCC</v>
       </c>
       <c r="D10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>Bioenergy</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -2664,43 +2796,43 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>Wind onshore</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>Wind offshore</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>Geothermal</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -2712,7 +2844,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -2724,102 +2856,102 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>Hydro pumped stg</v>
       </c>
       <c r="D18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>Util Batt Stg</v>
       </c>
       <c r="D19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>EV Batt</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E22" t="s">
+        <v>160</v>
+      </c>
+      <c r="F22" t="s">
         <v>161</v>
-      </c>
-      <c r="F22" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -2827,46 +2959,46 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" t="s">
         <v>107</v>
-      </c>
-      <c r="C26" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" t="s">
         <v>119</v>
-      </c>
-      <c r="C27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" t="s">
         <v>126</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>127</v>
-      </c>
-      <c r="C28" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B29" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" t="s">
         <v>129</v>
-      </c>
-      <c r="C29" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2894,33 +3026,33 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
       <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
         <v>78</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
         <v>79</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>81</v>
-      </c>
-      <c r="G2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H2" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CHE model - 2025-08-19 22:14
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE/ReportDefs_vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F722313C-51C9-4AE2-9912-CBFFFD05F5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B57AB34-5327-4613-BD06-2FC1B690AD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,15 @@
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
     <sheet name="TS_Defs" sheetId="27" r:id="rId2"/>
     <sheet name="TS_ratios" sheetId="68" r:id="rId3"/>
-    <sheet name="PSet_MAP coarse" sheetId="57" r:id="rId4"/>
-    <sheet name="CSET_MAP" sheetId="66" r:id="rId5"/>
-    <sheet name="CName_MAP" sheetId="58" r:id="rId6"/>
-    <sheet name="timeslice map" sheetId="64" r:id="rId7"/>
-    <sheet name="process map" sheetId="65" r:id="rId8"/>
-    <sheet name="commodity map" sheetId="67" r:id="rId9"/>
-    <sheet name="ATS" sheetId="63" r:id="rId10"/>
-    <sheet name="UnitConv" sheetId="59" r:id="rId11"/>
+    <sheet name="Sankey" sheetId="69" r:id="rId4"/>
+    <sheet name="PSet_MAP" sheetId="57" r:id="rId5"/>
+    <sheet name="CSET_MAP" sheetId="66" r:id="rId6"/>
+    <sheet name="CName_MAP" sheetId="58" r:id="rId7"/>
+    <sheet name="timeslice map" sheetId="64" r:id="rId8"/>
+    <sheet name="process map" sheetId="65" r:id="rId9"/>
+    <sheet name="commodity map" sheetId="67" r:id="rId10"/>
+    <sheet name="ATS" sheetId="63" r:id="rId11"/>
+    <sheet name="UnitConv" sheetId="59" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TS_Defs!$A$2:$N$2</definedName>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="257">
   <si>
     <t>Unit</t>
   </si>
@@ -91,12 +92,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Hydro</t>
-  </si>
-  <si>
-    <t>Nuclear</t>
-  </si>
-  <si>
     <t>Solar</t>
   </si>
   <si>
@@ -379,15 +374,9 @@
     <t>Wind offshore</t>
   </si>
   <si>
-    <t>Geothermal</t>
-  </si>
-  <si>
     <t>Hydro pumped stg</t>
   </si>
   <si>
-    <t>Bioenergy</t>
-  </si>
-  <si>
     <t>Util Batt Stg</t>
   </si>
   <si>
@@ -451,9 +440,6 @@
     <t>-ElcAgg*,-*EV*</t>
   </si>
   <si>
-    <t>ELC,ELC_???-???</t>
-  </si>
-  <si>
     <t>t</t>
   </si>
   <si>
@@ -487,160 +473,385 @@
     <t>timeslice</t>
   </si>
   <si>
-    <t>Delayed transition</t>
-  </si>
-  <si>
-    <t>Net Zero 2050</t>
+    <t>Low demand</t>
+  </si>
+  <si>
+    <t>Fragmented World</t>
+  </si>
+  <si>
+    <t>3 days</t>
+  </si>
+  <si>
+    <t>15 days</t>
+  </si>
+  <si>
+    <t>2 weeks</t>
+  </si>
+  <si>
+    <t>_3d</t>
+  </si>
+  <si>
+    <t>_15d</t>
+  </si>
+  <si>
+    <t>_2w</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>CO2Captured</t>
+  </si>
+  <si>
+    <t>kt</t>
+  </si>
+  <si>
+    <t>ktneg</t>
+  </si>
+  <si>
+    <t>CO2_emission</t>
+  </si>
+  <si>
+    <t>CO2_captured</t>
+  </si>
+  <si>
+    <t>mt</t>
+  </si>
+  <si>
+    <t>Coal CCS</t>
+  </si>
+  <si>
+    <t>Gas CCS</t>
+  </si>
+  <si>
+    <t>Coal CCS Retrofit</t>
+  </si>
+  <si>
+    <t>Gas CCS Retrofit</t>
+  </si>
+  <si>
+    <t>coal</t>
+  </si>
+  <si>
+    <t>gas</t>
+  </si>
+  <si>
+    <t>co2captured</t>
+  </si>
+  <si>
+    <t>*ccs-rf</t>
+  </si>
+  <si>
+    <t>co2net</t>
+  </si>
+  <si>
+    <t>000$/t</t>
+  </si>
+  <si>
+    <t>Price_CO2</t>
+  </si>
+  <si>
+    <t>$/tCO2</t>
+  </si>
+  <si>
+    <t>ELE,STG,IRE,-Grid</t>
+  </si>
+  <si>
+    <t>s?a*</t>
+  </si>
+  <si>
+    <t>*,-s?a*</t>
+  </si>
+  <si>
+    <t>hourly</t>
+  </si>
+  <si>
+    <t>aggregated</t>
+  </si>
+  <si>
+    <t>ts_type</t>
+  </si>
+  <si>
+    <t>ts_season</t>
+  </si>
+  <si>
+    <t>S1*</t>
+  </si>
+  <si>
+    <t>S2*</t>
+  </si>
+  <si>
+    <t>S3*</t>
+  </si>
+  <si>
+    <t>S4*</t>
+  </si>
+  <si>
+    <t>S5*</t>
+  </si>
+  <si>
+    <t>S6*</t>
+  </si>
+  <si>
+    <t>~Timeslice_Map</t>
+  </si>
+  <si>
+    <t>vstacks_ts16~</t>
+  </si>
+  <si>
+    <t>vstacks_t_annual~</t>
+  </si>
+  <si>
+    <t>ts-16</t>
+  </si>
+  <si>
+    <t>ts-annual</t>
+  </si>
+  <si>
+    <t>_16</t>
+  </si>
+  <si>
+    <t>_ann</t>
+  </si>
+  <si>
+    <t>-ElcAgg*,-*EV*,-g[_]*</t>
+  </si>
+  <si>
+    <t>ELC,ELC_???-???,e[_]*</t>
+  </si>
+  <si>
+    <t>T_neg_andor</t>
+  </si>
+  <si>
+    <t>downscale_option</t>
+  </si>
+  <si>
+    <t>~TS_Defs: Snk_attr=Grid Flows</t>
+  </si>
+  <si>
+    <t>TWh</t>
+  </si>
+  <si>
+    <t>VAR_FIN</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>Elec-220V</t>
+  </si>
+  <si>
+    <t>Elec-400V</t>
+  </si>
+  <si>
+    <t>Elec-380V</t>
+  </si>
+  <si>
+    <t>Elec-225V</t>
+  </si>
+  <si>
+    <t>Elec-330V</t>
+  </si>
+  <si>
+    <t>Elec-275V</t>
+  </si>
+  <si>
+    <t>Elec-420V</t>
+  </si>
+  <si>
+    <t>Elec-300V</t>
+  </si>
+  <si>
+    <t>Elec-500V</t>
+  </si>
+  <si>
+    <t>Elec-750V</t>
+  </si>
+  <si>
+    <t>Elec-450V</t>
+  </si>
+  <si>
+    <t>Elec-515V</t>
+  </si>
+  <si>
+    <t>Elec-525V</t>
+  </si>
+  <si>
+    <t>Elec-320V</t>
+  </si>
+  <si>
+    <t>Elec-150V</t>
+  </si>
+  <si>
+    <t>Elec-270V</t>
+  </si>
+  <si>
+    <t>Elec-350V</t>
+  </si>
+  <si>
+    <t>Elec-250V</t>
+  </si>
+  <si>
+    <t>Elec-200V</t>
+  </si>
+  <si>
+    <t>Elec-236V</t>
+  </si>
+  <si>
+    <t>Elec-600V</t>
+  </si>
+  <si>
+    <t>bioenergy</t>
+  </si>
+  <si>
+    <t>hydrogen</t>
+  </si>
+  <si>
+    <t>nuclear</t>
+  </si>
+  <si>
+    <t>ELC</t>
+  </si>
+  <si>
+    <t>buildings</t>
+  </si>
+  <si>
+    <t>industry</t>
+  </si>
+  <si>
+    <t>transport</t>
+  </si>
+  <si>
+    <t>EVs</t>
+  </si>
+  <si>
+    <t>&lt;cset&gt;_Src_&lt;pset&gt;</t>
+  </si>
+  <si>
+    <t>&lt;cset&gt;_Snk_&lt;pset&gt;</t>
+  </si>
+  <si>
+    <t>fossil</t>
+  </si>
+  <si>
+    <t>Bio Power</t>
+  </si>
+  <si>
+    <t>Solar Util</t>
+  </si>
+  <si>
+    <t>Geothermal P</t>
+  </si>
+  <si>
+    <t>Hydro RoR</t>
+  </si>
+  <si>
+    <t>Nuclear P</t>
+  </si>
+  <si>
+    <t>Nuclear SMR</t>
+  </si>
+  <si>
+    <t>Hydro Dam</t>
+  </si>
+  <si>
+    <t>Solar elec</t>
+  </si>
+  <si>
+    <t>Wind elec</t>
+  </si>
+  <si>
+    <t>renewable</t>
+  </si>
+  <si>
+    <t>Grid-220V</t>
+  </si>
+  <si>
+    <t>Grid-400V</t>
+  </si>
+  <si>
+    <t>Grid-380V</t>
+  </si>
+  <si>
+    <t>Grid-225V</t>
+  </si>
+  <si>
+    <t>Grid-330V</t>
+  </si>
+  <si>
+    <t>Grid-275V</t>
+  </si>
+  <si>
+    <t>Grid-420V</t>
+  </si>
+  <si>
+    <t>Grid-300V</t>
+  </si>
+  <si>
+    <t>Grid-500V</t>
+  </si>
+  <si>
+    <t>Grid-750V</t>
+  </si>
+  <si>
+    <t>Grid-450V</t>
+  </si>
+  <si>
+    <t>Grid-515V</t>
+  </si>
+  <si>
+    <t>Grid-525V</t>
+  </si>
+  <si>
+    <t>Grid-320V</t>
+  </si>
+  <si>
+    <t>Grid-150V</t>
+  </si>
+  <si>
+    <t>Grid-270V</t>
+  </si>
+  <si>
+    <t>Grid-350V</t>
+  </si>
+  <si>
+    <t>Grid-250V</t>
+  </si>
+  <si>
+    <t>Grid-200V</t>
+  </si>
+  <si>
+    <t>Grid-236V</t>
+  </si>
+  <si>
+    <t>Grid-600V</t>
+  </si>
+  <si>
+    <t>Aggregators</t>
+  </si>
+  <si>
+    <t>DUMMY_IMP</t>
+  </si>
+  <si>
+    <t>Transformers Dn</t>
+  </si>
+  <si>
+    <t>Transformers Up</t>
+  </si>
+  <si>
+    <t>Declared NDCs</t>
+  </si>
+  <si>
+    <t>Limited to 2 deg</t>
+  </si>
+  <si>
+    <t>Postponed Transition</t>
+  </si>
+  <si>
+    <t>Target Net Zero 2050</t>
   </si>
   <si>
     <t>Current Policies</t>
-  </si>
-  <si>
-    <t>Low demand</t>
-  </si>
-  <si>
-    <t>Fragmented World</t>
-  </si>
-  <si>
-    <t>NDCs</t>
-  </si>
-  <si>
-    <t>Below 2deg</t>
-  </si>
-  <si>
-    <t>3 days</t>
-  </si>
-  <si>
-    <t>15 days</t>
-  </si>
-  <si>
-    <t>2 weeks</t>
-  </si>
-  <si>
-    <t>_3d</t>
-  </si>
-  <si>
-    <t>_15d</t>
-  </si>
-  <si>
-    <t>_2w</t>
-  </si>
-  <si>
-    <t>CO2</t>
-  </si>
-  <si>
-    <t>CO2Captured</t>
-  </si>
-  <si>
-    <t>kt</t>
-  </si>
-  <si>
-    <t>ktneg</t>
-  </si>
-  <si>
-    <t>CO2_emission</t>
-  </si>
-  <si>
-    <t>CO2_captured</t>
-  </si>
-  <si>
-    <t>mt</t>
-  </si>
-  <si>
-    <t>Coal CCS</t>
-  </si>
-  <si>
-    <t>Gas CCS</t>
-  </si>
-  <si>
-    <t>Coal CCS Retrofit</t>
-  </si>
-  <si>
-    <t>Gas CCS Retrofit</t>
-  </si>
-  <si>
-    <t>coal</t>
-  </si>
-  <si>
-    <t>gas</t>
-  </si>
-  <si>
-    <t>co2captured</t>
-  </si>
-  <si>
-    <t>*ccs-rf</t>
-  </si>
-  <si>
-    <t>co2net</t>
-  </si>
-  <si>
-    <t>000$/t</t>
-  </si>
-  <si>
-    <t>Price_CO2</t>
-  </si>
-  <si>
-    <t>$/tCO2</t>
-  </si>
-  <si>
-    <t>ELE,STG,IRE,-Grid</t>
-  </si>
-  <si>
-    <t>s?a*</t>
-  </si>
-  <si>
-    <t>*,-s?a*</t>
-  </si>
-  <si>
-    <t>hourly</t>
-  </si>
-  <si>
-    <t>aggregated</t>
-  </si>
-  <si>
-    <t>ts_type</t>
-  </si>
-  <si>
-    <t>ts_season</t>
-  </si>
-  <si>
-    <t>S1*</t>
-  </si>
-  <si>
-    <t>S2*</t>
-  </si>
-  <si>
-    <t>S3*</t>
-  </si>
-  <si>
-    <t>S4*</t>
-  </si>
-  <si>
-    <t>S5*</t>
-  </si>
-  <si>
-    <t>S6*</t>
-  </si>
-  <si>
-    <t>~Timeslice_Map</t>
-  </si>
-  <si>
-    <t>vstacks_ts16~</t>
-  </si>
-  <si>
-    <t>vstacks_t_annual~</t>
-  </si>
-  <si>
-    <t>ts-16</t>
-  </si>
-  <si>
-    <t>ts-annual</t>
-  </si>
-  <si>
-    <t>_16</t>
-  </si>
-  <si>
-    <t>_ann</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1399,7 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.73046875" defaultRowHeight="14.25"/>
@@ -1206,43 +1417,43 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D1" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="E1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="H2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="I2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -1251,10 +1462,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H5" t="str">
         <f>"sg_"&amp;H2</f>
@@ -1272,23 +1483,23 @@
       </c>
       <c r="B6" t="str">
         <f>G6</f>
-        <v>Delayed transition_3d</v>
+        <v>Postponed Transition_3d</v>
       </c>
       <c r="G6" t="str">
         <f>H6&amp;P6</f>
-        <v>Delayed transition_3d</v>
+        <v>Postponed Transition_3d</v>
       </c>
       <c r="H6" t="s">
-        <v>135</v>
+        <v>254</v>
       </c>
       <c r="I6" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1298,23 +1509,23 @@
       </c>
       <c r="B7" t="str">
         <f t="shared" ref="B7:B26" si="1">G7</f>
-        <v>Net Zero 2050_3d</v>
+        <v>Target Net Zero 2050_3d</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ref="G7:G26" si="2">H7&amp;P7</f>
-        <v>Net Zero 2050_3d</v>
+        <v>Target Net Zero 2050_3d</v>
       </c>
       <c r="H7" t="s">
-        <v>136</v>
+        <v>255</v>
       </c>
       <c r="I7" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N7">
         <v>2</v>
       </c>
       <c r="P7" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1324,23 +1535,23 @@
       </c>
       <c r="B8" t="str">
         <f t="shared" si="1"/>
-        <v>NDCs_3d</v>
+        <v>Declared NDCs_3d</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="2"/>
-        <v>NDCs_3d</v>
+        <v>Declared NDCs_3d</v>
       </c>
       <c r="H8" t="s">
-        <v>140</v>
+        <v>252</v>
       </c>
       <c r="I8" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N8">
         <v>3</v>
       </c>
       <c r="P8" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1350,23 +1561,23 @@
       </c>
       <c r="B9" t="str">
         <f t="shared" si="1"/>
-        <v>Below 2deg_3d</v>
+        <v>Limited to 2 deg_3d</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="2"/>
-        <v>Below 2deg_3d</v>
+        <v>Limited to 2 deg_3d</v>
       </c>
       <c r="H9" t="s">
-        <v>141</v>
+        <v>253</v>
       </c>
       <c r="I9" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N9">
         <v>4</v>
       </c>
       <c r="P9" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1383,16 +1594,16 @@
         <v>Current Policies_3d</v>
       </c>
       <c r="H10" t="s">
-        <v>137</v>
+        <v>256</v>
       </c>
       <c r="I10" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N10">
         <v>5</v>
       </c>
       <c r="P10" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1409,16 +1620,16 @@
         <v>Low demand_3d</v>
       </c>
       <c r="H11" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="I11" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N11">
         <v>6</v>
       </c>
       <c r="P11" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1435,16 +1646,16 @@
         <v>Fragmented World_3d</v>
       </c>
       <c r="H12" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="I12" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N12">
         <v>7</v>
       </c>
       <c r="P12" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1454,25 +1665,25 @@
       </c>
       <c r="B13" t="str">
         <f t="shared" si="1"/>
-        <v>Delayed transition_15d</v>
+        <v>Postponed Transition_15d</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="2"/>
-        <v>Delayed transition_15d</v>
+        <v>Postponed Transition_15d</v>
       </c>
       <c r="H13" t="str">
         <f>H6</f>
-        <v>Delayed transition</v>
+        <v>Postponed Transition</v>
       </c>
       <c r="I13" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N13">
         <f>N6</f>
         <v>1</v>
       </c>
       <c r="P13" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1482,25 +1693,25 @@
       </c>
       <c r="B14" t="str">
         <f t="shared" si="1"/>
-        <v>Net Zero 2050_15d</v>
+        <v>Target Net Zero 2050_15d</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="2"/>
-        <v>Net Zero 2050_15d</v>
+        <v>Target Net Zero 2050_15d</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" ref="H14:H41" si="4">H7</f>
-        <v>Net Zero 2050</v>
+        <f t="shared" ref="H14:H40" si="4">H7</f>
+        <v>Target Net Zero 2050</v>
       </c>
       <c r="I14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N14">
         <f t="shared" ref="N14:N40" si="5">N7</f>
         <v>2</v>
       </c>
       <c r="P14" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1510,25 +1721,25 @@
       </c>
       <c r="B15" t="str">
         <f t="shared" si="1"/>
-        <v>NDCs_15d</v>
+        <v>Declared NDCs_15d</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="2"/>
-        <v>NDCs_15d</v>
+        <v>Declared NDCs_15d</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="4"/>
-        <v>NDCs</v>
+        <v>Declared NDCs</v>
       </c>
       <c r="I15" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N15">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P15" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1538,25 +1749,25 @@
       </c>
       <c r="B16" t="str">
         <f t="shared" si="1"/>
-        <v>Below 2deg_15d</v>
+        <v>Limited to 2 deg_15d</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="2"/>
-        <v>Below 2deg_15d</v>
+        <v>Limited to 2 deg_15d</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="4"/>
-        <v>Below 2deg</v>
+        <v>Limited to 2 deg</v>
       </c>
       <c r="I16" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N16">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P16" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1577,14 +1788,14 @@
         <v>Current Policies</v>
       </c>
       <c r="I17" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N17">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P17" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1605,14 +1816,14 @@
         <v>Low demand</v>
       </c>
       <c r="I18" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N18">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P18" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1633,14 +1844,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I19" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N19">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P19" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1650,25 +1861,25 @@
       </c>
       <c r="B20" t="str">
         <f t="shared" si="1"/>
-        <v>Delayed transition_2w</v>
+        <v>Postponed Transition_2w</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="2"/>
-        <v>Delayed transition_2w</v>
+        <v>Postponed Transition_2w</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="4"/>
-        <v>Delayed transition</v>
+        <v>Postponed Transition</v>
       </c>
       <c r="I20" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N20">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P20" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1678,25 +1889,25 @@
       </c>
       <c r="B21" t="str">
         <f t="shared" si="1"/>
-        <v>Net Zero 2050_2w</v>
+        <v>Target Net Zero 2050_2w</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="2"/>
-        <v>Net Zero 2050_2w</v>
+        <v>Target Net Zero 2050_2w</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="4"/>
-        <v>Net Zero 2050</v>
+        <v>Target Net Zero 2050</v>
       </c>
       <c r="I21" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N21">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="P21" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1706,25 +1917,25 @@
       </c>
       <c r="B22" t="str">
         <f t="shared" si="1"/>
-        <v>NDCs_2w</v>
+        <v>Declared NDCs_2w</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="2"/>
-        <v>NDCs_2w</v>
+        <v>Declared NDCs_2w</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="4"/>
-        <v>NDCs</v>
+        <v>Declared NDCs</v>
       </c>
       <c r="I22" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P22" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1734,25 +1945,25 @@
       </c>
       <c r="B23" t="str">
         <f t="shared" si="1"/>
-        <v>Below 2deg_2w</v>
+        <v>Limited to 2 deg_2w</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="2"/>
-        <v>Below 2deg_2w</v>
+        <v>Limited to 2 deg_2w</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="4"/>
-        <v>Below 2deg</v>
+        <v>Limited to 2 deg</v>
       </c>
       <c r="I23" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N23">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P23" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1773,14 +1984,14 @@
         <v>Current Policies</v>
       </c>
       <c r="I24" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N24">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P24" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1801,14 +2012,14 @@
         <v>Low demand</v>
       </c>
       <c r="I25" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N25">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P25" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -1829,14 +2040,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I26" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N26">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P26" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -1845,54 +2056,54 @@
         <v>vstacks_ts16~0001</v>
       </c>
       <c r="B27" t="str">
-        <f t="shared" ref="B27:B41" si="7">G27</f>
-        <v>Delayed transition_16</v>
+        <f t="shared" ref="B27:B40" si="7">G27</f>
+        <v>Postponed Transition_16</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" ref="G27:G41" si="8">H27&amp;P27</f>
-        <v>Delayed transition_16</v>
+        <f t="shared" ref="G27:G40" si="8">H27&amp;P27</f>
+        <v>Postponed Transition_16</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="4"/>
-        <v>Delayed transition</v>
+        <v>Postponed Transition</v>
       </c>
       <c r="I27" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="N27">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P27" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" t="str">
-        <f t="shared" ref="A28:A40" si="9">$D$1&amp;TEXT(N28,"0000")</f>
+        <f t="shared" ref="A28:A33" si="9">$D$1&amp;TEXT(N28,"0000")</f>
         <v>vstacks_ts16~0002</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="7"/>
-        <v>Net Zero 2050_16</v>
+        <v>Target Net Zero 2050_16</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="8"/>
-        <v>Net Zero 2050_16</v>
+        <v>Target Net Zero 2050_16</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="4"/>
-        <v>Net Zero 2050</v>
+        <v>Target Net Zero 2050</v>
       </c>
       <c r="I28" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="N28">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="P28" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -1902,25 +2113,25 @@
       </c>
       <c r="B29" t="str">
         <f t="shared" si="7"/>
-        <v>NDCs_16</v>
+        <v>Declared NDCs_16</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="8"/>
-        <v>NDCs_16</v>
+        <v>Declared NDCs_16</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="4"/>
-        <v>NDCs</v>
+        <v>Declared NDCs</v>
       </c>
       <c r="I29" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="N29">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P29" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -1930,25 +2141,25 @@
       </c>
       <c r="B30" t="str">
         <f t="shared" si="7"/>
-        <v>Below 2deg_16</v>
+        <v>Limited to 2 deg_16</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="8"/>
-        <v>Below 2deg_16</v>
+        <v>Limited to 2 deg_16</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="4"/>
-        <v>Below 2deg</v>
+        <v>Limited to 2 deg</v>
       </c>
       <c r="I30" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="N30">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P30" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -1969,14 +2180,14 @@
         <v>Current Policies</v>
       </c>
       <c r="I31" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="N31">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P31" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -1997,14 +2208,14 @@
         <v>Low demand</v>
       </c>
       <c r="I32" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="N32">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P32" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -2025,14 +2236,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I33" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="N33">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P33" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -2042,25 +2253,25 @@
       </c>
       <c r="B34" t="str">
         <f t="shared" si="7"/>
-        <v>Delayed transition_ann</v>
+        <v>Postponed Transition_ann</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="8"/>
-        <v>Delayed transition_ann</v>
+        <v>Postponed Transition_ann</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="4"/>
-        <v>Delayed transition</v>
+        <v>Postponed Transition</v>
       </c>
       <c r="I34" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="N34">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P34" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -2070,25 +2281,25 @@
       </c>
       <c r="B35" t="str">
         <f t="shared" si="7"/>
-        <v>Net Zero 2050_ann</v>
+        <v>Target Net Zero 2050_ann</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="8"/>
-        <v>Net Zero 2050_ann</v>
+        <v>Target Net Zero 2050_ann</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="4"/>
-        <v>Net Zero 2050</v>
+        <v>Target Net Zero 2050</v>
       </c>
       <c r="I35" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="N35">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="P35" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -2098,25 +2309,25 @@
       </c>
       <c r="B36" t="str">
         <f t="shared" si="7"/>
-        <v>NDCs_ann</v>
+        <v>Declared NDCs_ann</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="8"/>
-        <v>NDCs_ann</v>
+        <v>Declared NDCs_ann</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="4"/>
-        <v>NDCs</v>
+        <v>Declared NDCs</v>
       </c>
       <c r="I36" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="N36">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P36" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -2126,25 +2337,25 @@
       </c>
       <c r="B37" t="str">
         <f t="shared" si="7"/>
-        <v>Below 2deg_ann</v>
+        <v>Limited to 2 deg_ann</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="8"/>
-        <v>Below 2deg_ann</v>
+        <v>Limited to 2 deg_ann</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="4"/>
-        <v>Below 2deg</v>
+        <v>Limited to 2 deg</v>
       </c>
       <c r="I37" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="N37">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P37" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -2165,14 +2376,14 @@
         <v>Current Policies</v>
       </c>
       <c r="I38" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="N38">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P38" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -2193,14 +2404,14 @@
         <v>Low demand</v>
       </c>
       <c r="I39" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="N39">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P39" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -2221,14 +2432,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I40" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="N40">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P40" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2239,6 +2450,60 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3245E1-8745-41DD-8AE6-2F4FA19D9F1C}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G3"/>
@@ -2252,30 +2517,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2286,7 +2551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet31"/>
   <dimension ref="A1:D7"/>
@@ -2310,32 +2575,32 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <f>1/8.76</f>
@@ -2344,13 +2609,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D4">
         <f>1/8.76*100</f>
@@ -2359,13 +2624,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C5" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D5">
         <v>1E-3</v>
@@ -2373,13 +2638,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D6">
         <v>-1E-3</v>
@@ -2387,13 +2652,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D7">
         <v>-1000</v>
@@ -2411,7 +2676,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -2442,48 +2707,48 @@
   <sheetData>
     <row r="1" spans="1:21" ht="17.25" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15" thickTop="1" thickBot="1">
       <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="E2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>2</v>
@@ -2492,226 +2757,226 @@
         <v>1</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>122</v>
+        <v>177</v>
       </c>
       <c r="K3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>122</v>
+        <v>177</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="U4" s="8"/>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>122</v>
+        <v>177</v>
       </c>
       <c r="I5" t="s">
-        <v>123</v>
+        <v>178</v>
       </c>
       <c r="K5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="N5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="D6" s="2"/>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="K7" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="N7" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="K8" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="N8" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N10" t="s">
+        <v>46</v>
+      </c>
+      <c r="P10" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q10" t="s">
         <v>48</v>
-      </c>
-      <c r="P10" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="K11" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="N11" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" t="s">
+        <v>85</v>
+      </c>
+      <c r="N12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P12" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q12" t="s">
         <v>51</v>
-      </c>
-      <c r="K12" t="s">
-        <v>87</v>
-      </c>
-      <c r="N12" t="s">
-        <v>52</v>
-      </c>
-      <c r="P12" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2746,15 +3011,15 @@
   <sheetData>
     <row r="1" spans="3:11">
       <c r="C1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="3:11">
       <c r="C2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -2763,42 +3028,42 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="J2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="3:11">
       <c r="C3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="J3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2809,35 +3074,584 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D44EBE-400A-4EA2-9DA1-076783A77DFC}">
+  <dimension ref="A3:S6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="30.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="255.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.53125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.53125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.9296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:19" ht="17.25" thickBot="1">
+      <c r="A3" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15" thickTop="1" thickBot="1">
+      <c r="A4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,PSet_MAP!$A$3:$A$49)</f>
+        <v>CCGT,Int Comb,Gas_Oil Steam,OCGT (Peaker),Subcritical Coal,Supercritical Coal,IGCC,Bio Power,Solar Util,Wind onshore,Wind offshore,Geothermal P,Hydro Dam,Hydro RoR,Nuclear P,Nuclear SMR,Hydro pumped stg,Util Batt Stg,EV Batt,Demand,Transformers Dn,Transformers Up,Grid-220V,Grid-400V,Grid-380V,Grid-225V,Grid-330V,Grid-275V,Grid-420V,Grid-300V,Grid-500V,Grid-750V,Grid-450V,Grid-515V,Grid-525V,Grid-320V,Grid-150V,Grid-270V,Grid-350V,Grid-250V,Grid-200V,Grid-236V,Grid-600V,Aggregators,DUMMY_IMP</v>
+      </c>
+      <c r="G5" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,CSET_MAP!$A$3:$A$43)</f>
+        <v>Elec-220V,Elec-400V,Elec-380V,Elec-225V,Elec-330V,Elec-275V,Elec-420V,Elec-300V,Elec-500V,Elec-750V,Elec-450V,Elec-515V,Elec-525V,Elec-320V,Elec-150V,Elec-270V,Elec-350V,Elec-250V,Elec-200V,Elec-236V,Elec-600V,Solar elec,Wind elec,fossil,renewable,bioenergy,hydrogen,nuclear,ELC,buildings,industry,transport,EVs</v>
+      </c>
+      <c r="J5" t="s">
+        <v>182</v>
+      </c>
+      <c r="M5" t="s">
+        <v>214</v>
+      </c>
+      <c r="S5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,PSet_MAP!$A$3:$A$49)</f>
+        <v>CCGT,Int Comb,Gas_Oil Steam,OCGT (Peaker),Subcritical Coal,Supercritical Coal,IGCC,Bio Power,Solar Util,Wind onshore,Wind offshore,Geothermal P,Hydro Dam,Hydro RoR,Nuclear P,Nuclear SMR,Hydro pumped stg,Util Batt Stg,EV Batt,Demand,Transformers Dn,Transformers Up,Grid-220V,Grid-400V,Grid-380V,Grid-225V,Grid-330V,Grid-275V,Grid-420V,Grid-300V,Grid-500V,Grid-750V,Grid-450V,Grid-515V,Grid-525V,Grid-320V,Grid-150V,Grid-270V,Grid-350V,Grid-250V,Grid-200V,Grid-236V,Grid-600V,Aggregators,DUMMY_IMP</v>
+      </c>
+      <c r="G6" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,CSET_MAP!$A$3:$A$43)</f>
+        <v>Elec-220V,Elec-400V,Elec-380V,Elec-225V,Elec-330V,Elec-275V,Elec-420V,Elec-300V,Elec-500V,Elec-750V,Elec-450V,Elec-515V,Elec-525V,Elec-320V,Elec-150V,Elec-270V,Elec-350V,Elec-250V,Elec-200V,Elec-236V,Elec-600V,Solar elec,Wind elec,fossil,renewable,bioenergy,hydrogen,nuclear,ELC,buildings,industry,transport,EVs</v>
+      </c>
+      <c r="J6" t="s">
+        <v>182</v>
+      </c>
+      <c r="M6" t="s">
+        <v>215</v>
+      </c>
+      <c r="S6">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.265625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="str">
+        <f>A3</f>
+        <v>CCGT</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B47" si="0">A4</f>
+        <v>Int Comb</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Gas_Oil Steam</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>OCGT (Peaker)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>Subcritical Coal</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>Supercritical Coal</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>IGCC</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>Bio Power</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>Solar Util</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>Wind onshore</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>Wind offshore</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>Geothermal P</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>Hydro Dam</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>220</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>Hydro RoR</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>Nuclear P</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>Nuclear SMR</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>Hydro pumped stg</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>Util Batt Stg</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>EV Batt</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>Demand</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>250</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>Transformers Dn</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>251</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>Transformers Up</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>227</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-220V</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>228</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-400V</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>229</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-380V</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>230</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-225V</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>231</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-330V</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>232</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-275V</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>233</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-420V</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>234</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-300V</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>235</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-500V</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>236</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-750V</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>237</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-450V</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>238</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-515V</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>239</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-525V</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>240</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-320V</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>241</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-150V</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>242</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-270V</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>243</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-350V</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>244</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-250V</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>245</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-200V</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>246</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-236V</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>247</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-600V</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>248</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>Aggregators</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>249</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>DUMMY_IMP</v>
       </c>
     </row>
   </sheetData>
@@ -2846,12 +3660,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E766D8-7F73-4A5A-98A5-9C85D527817F}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2861,18 +3675,315 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" t="str">
+        <f>A3</f>
+        <v>Elec-220V</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B35" si="0">A4</f>
+        <v>Elec-400V</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-380V</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-225V</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-330V</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-275V</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-420V</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-300V</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-500V</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-750V</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-450V</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-515V</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>197</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-525V</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>198</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-320V</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-150V</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>200</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-270V</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>201</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-350V</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-250V</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>203</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-200V</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>204</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-236V</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>205</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-600V</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>224</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>Solar elec</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>225</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>Wind elec</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>216</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>fossil</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>226</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>renewable</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>206</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>bioenergy</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>207</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>hydrogen</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>208</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>nuclear</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>209</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>ELC</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>210</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>buildings</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>211</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>industry</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>212</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>transport</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>213</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>EVs</v>
       </c>
     </row>
   </sheetData>
@@ -2880,7 +3991,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C2"/>
@@ -2900,18 +4011,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2920,7 +4031,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32957E82-8232-40A9-A839-CC5F79005B92}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C10"/>
@@ -2938,48 +4049,48 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C5" t="str">
         <f>LEFT(B5,2)</f>
@@ -2988,10 +4099,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ref="C6:C10" si="0">LEFT(B6,2)</f>
@@ -3000,10 +4111,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -3012,10 +4123,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -3024,10 +4135,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -3036,10 +4147,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B10" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -3051,12 +4162,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10ADB714-E6AA-4E3E-B77B-62B65BA0E218}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3071,411 +4182,681 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17.25" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1" thickBot="1">
       <c r="A2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="D2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" t="str">
-        <f>D3</f>
-        <v>CCGT</v>
-      </c>
-      <c r="D3" t="s">
-        <v>90</v>
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" ref="C4:C20" si="0">D4</f>
-        <v>Int Comb</v>
-      </c>
-      <c r="D4" t="s">
-        <v>91</v>
+        <v>120</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>Gas_Oil Steam</v>
+        <f>D5</f>
+        <v>CCGT</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>Nuclear</v>
+        <f t="shared" ref="C6:C49" si="0">D6</f>
+        <v>Int Comb</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>OCGT (Peaker)</v>
+        <v>Gas_Oil Steam</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>Subcritical Coal</v>
+        <v>OCGT (Peaker)</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>Supercritical Coal</v>
+        <v>Subcritical Coal</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>IGCC</v>
+        <v>Supercritical Coal</v>
       </c>
       <c r="D10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>Bioenergy</v>
+        <v>IGCC</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>Solar</v>
+        <v>Bio Power</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>Wind onshore</v>
+        <v>Solar Util</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>Wind offshore</v>
+        <v>Wind onshore</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>Geothermal</v>
+        <v>Wind offshore</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>Hydro</v>
+        <v>Geothermal P</v>
       </c>
       <c r="D16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>Hydro Dam</v>
+      </c>
+      <c r="D17" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>Hydro RoR</v>
+      </c>
+      <c r="D18" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>Nuclear P</v>
+      </c>
+      <c r="D19" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>Nuclear SMR</v>
+      </c>
+      <c r="D20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>Hydro pumped stg</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>Util Batt Stg</v>
+      </c>
+      <c r="D22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>EV Batt</v>
+      </c>
+      <c r="D23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>Demand</v>
+      </c>
+      <c r="D24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>Transformers Dn</v>
+      </c>
+      <c r="D25" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>Transformers Up</v>
+      </c>
+      <c r="D26" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-220V</v>
+      </c>
+      <c r="D27" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-400V</v>
+      </c>
+      <c r="D28" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-380V</v>
+      </c>
+      <c r="D29" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-225V</v>
+      </c>
+      <c r="D30" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-330V</v>
+      </c>
+      <c r="D31" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-275V</v>
+      </c>
+      <c r="D32" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-420V</v>
+      </c>
+      <c r="D33" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-300V</v>
+      </c>
+      <c r="D34" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-500V</v>
+      </c>
+      <c r="D35" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-750V</v>
+      </c>
+      <c r="D36" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-450V</v>
+      </c>
+      <c r="D37" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-515V</v>
+      </c>
+      <c r="D38" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-525V</v>
+      </c>
+      <c r="D39" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-320V</v>
+      </c>
+      <c r="D40" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-150V</v>
+      </c>
+      <c r="D41" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-270V</v>
+      </c>
+      <c r="D42" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-350V</v>
+      </c>
+      <c r="D43" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-250V</v>
+      </c>
+      <c r="D44" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-200V</v>
+      </c>
+      <c r="D45" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-236V</v>
+      </c>
+      <c r="D46" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-600V</v>
+      </c>
+      <c r="D47" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>Aggregators</v>
+      </c>
+      <c r="D48" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>DUMMY_IMP</v>
+      </c>
+      <c r="D49" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" t="s">
+        <v>145</v>
+      </c>
+      <c r="E50" t="s">
+        <v>149</v>
+      </c>
+      <c r="F50" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" t="s">
+        <v>150</v>
+      </c>
+      <c r="F51" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" t="s">
+        <v>152</v>
+      </c>
+      <c r="C53" t="s">
+        <v>148</v>
+      </c>
+      <c r="E53" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>Nuclear</v>
-      </c>
-      <c r="D17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v>Hydro pumped stg</v>
-      </c>
-      <c r="D18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v>Util Batt Stg</v>
-      </c>
-      <c r="D19" t="s">
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>EV Batt</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C55" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" t="s">
-        <v>155</v>
-      </c>
-      <c r="E21" t="s">
-        <v>159</v>
-      </c>
-      <c r="F21" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" t="s">
-        <v>156</v>
-      </c>
-      <c r="E22" t="s">
-        <v>160</v>
-      </c>
-      <c r="F22" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C23" t="s">
-        <v>157</v>
-      </c>
-      <c r="E23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" t="s">
-        <v>162</v>
-      </c>
-      <c r="C24" t="s">
-        <v>158</v>
-      </c>
-      <c r="E24" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" t="s">
-        <v>118</v>
-      </c>
-      <c r="C27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>125</v>
-      </c>
-      <c r="B28" t="s">
-        <v>126</v>
-      </c>
-      <c r="C28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>125</v>
-      </c>
-      <c r="B29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C29" t="s">
-        <v>129</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3245E1-8745-41DD-8AE6-2F4FA19D9F1C}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" t="s">
-        <v>81</v>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CHE model - 2025-08-31 22:13
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_CHE/ReportDefs_vervestacks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B57AB34-5327-4613-BD06-2FC1B690AD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3E5D9C-1147-474B-8198-75F0DCCCD524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="265">
   <si>
     <t>Unit</t>
   </si>
@@ -458,45 +458,9 @@
     <t>old</t>
   </si>
   <si>
-    <t>vstacks_t1~</t>
-  </si>
-  <si>
-    <t>vstacks_t5~</t>
-  </si>
-  <si>
-    <t>vstacks_w2~</t>
-  </si>
-  <si>
-    <t>ngfs</t>
-  </si>
-  <si>
     <t>timeslice</t>
   </si>
   <si>
-    <t>Low demand</t>
-  </si>
-  <si>
-    <t>Fragmented World</t>
-  </si>
-  <si>
-    <t>3 days</t>
-  </si>
-  <si>
-    <t>15 days</t>
-  </si>
-  <si>
-    <t>2 weeks</t>
-  </si>
-  <si>
-    <t>_3d</t>
-  </si>
-  <si>
-    <t>_15d</t>
-  </si>
-  <si>
-    <t>_2w</t>
-  </si>
-  <si>
     <t>CO2</t>
   </si>
   <si>
@@ -536,9 +500,6 @@
     <t>gas</t>
   </si>
   <si>
-    <t>co2captured</t>
-  </si>
-  <si>
     <t>*ccs-rf</t>
   </si>
   <si>
@@ -596,30 +557,9 @@
     <t>~Timeslice_Map</t>
   </si>
   <si>
-    <t>vstacks_ts16~</t>
-  </si>
-  <si>
-    <t>vstacks_t_annual~</t>
-  </si>
-  <si>
-    <t>ts-16</t>
-  </si>
-  <si>
-    <t>ts-annual</t>
-  </si>
-  <si>
-    <t>_16</t>
-  </si>
-  <si>
-    <t>_ann</t>
-  </si>
-  <si>
     <t>-ElcAgg*,-*EV*,-g[_]*</t>
   </si>
   <si>
-    <t>ELC,ELC_???-???,e[_]*</t>
-  </si>
-  <si>
     <t>T_neg_andor</t>
   </si>
   <si>
@@ -839,19 +779,103 @@
     <t>Transformers Up</t>
   </si>
   <si>
-    <t>Declared NDCs</t>
-  </si>
-  <si>
-    <t>Limited to 2 deg</t>
-  </si>
-  <si>
-    <t>Postponed Transition</t>
-  </si>
-  <si>
-    <t>Target Net Zero 2050</t>
-  </si>
-  <si>
-    <t>Current Policies</t>
+    <t>s1p1v1_d</t>
+  </si>
+  <si>
+    <t>s3p3v3_d</t>
+  </si>
+  <si>
+    <t>s2_w</t>
+  </si>
+  <si>
+    <t>s2_w_p2_d</t>
+  </si>
+  <si>
+    <t>ts12_clu</t>
+  </si>
+  <si>
+    <t>ts24_clu</t>
+  </si>
+  <si>
+    <t>ts48_clu</t>
+  </si>
+  <si>
+    <t>s5p5v5_d</t>
+  </si>
+  <si>
+    <t>ts_annual</t>
+  </si>
+  <si>
+    <t>ts_12</t>
+  </si>
+  <si>
+    <t>a2w2d</t>
+  </si>
+  <si>
+    <t>d9d</t>
+  </si>
+  <si>
+    <t>b2w</t>
+  </si>
+  <si>
+    <t>c15d</t>
+  </si>
+  <si>
+    <t>e3d</t>
+  </si>
+  <si>
+    <t>fTS48c</t>
+  </si>
+  <si>
+    <t>gTS24c</t>
+  </si>
+  <si>
+    <t>hTS12c</t>
+  </si>
+  <si>
+    <t>iTS12</t>
+  </si>
+  <si>
+    <t>jAnn</t>
+  </si>
+  <si>
+    <t>Limit warming to 1.5°C (&gt;50%) with no or limited overshoot</t>
+  </si>
+  <si>
+    <t>Limit warming to 1.5°C (&gt;67%) with high overshoot</t>
+  </si>
+  <si>
+    <t>Limit warming to 2°C (&gt;67%) with higher action post-2030</t>
+  </si>
+  <si>
+    <t>Limit warming to 2°C (&gt;50%) with immediate action</t>
+  </si>
+  <si>
+    <t>Likely above 3°C warming with limited mitigation</t>
+  </si>
+  <si>
+    <t>b 2 deg (50%)</t>
+  </si>
+  <si>
+    <t>c 2 deg (67%)</t>
+  </si>
+  <si>
+    <t>d 1.5 deg OS</t>
+  </si>
+  <si>
+    <t>e 1.5 deg no OS</t>
+  </si>
+  <si>
+    <t>a 3 deg</t>
+  </si>
+  <si>
+    <t>ar6_r10</t>
+  </si>
+  <si>
+    <t>ELC,ELC_???-???*,e[_]*</t>
+  </si>
+  <si>
+    <t>*ccs</t>
   </si>
 </sst>
 </file>
@@ -1396,1053 +1420,1868 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.73046875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.73046875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="1.73046875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21">
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="I2" t="s">
+        <v>262</v>
+      </c>
+      <c r="J2" t="s">
         <v>125</v>
       </c>
-      <c r="B1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E1" t="s">
-        <v>172</v>
-      </c>
-      <c r="H1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="H2" t="s">
-        <v>128</v>
-      </c>
-      <c r="I2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:21">
+      <c r="B4" t="s">
         <v>63</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>9</v>
-      </c>
-      <c r="H5" t="str">
-        <f>"sg_"&amp;H2</f>
-        <v>sg_ngfs</v>
       </c>
       <c r="I5" t="str">
         <f>"sg_"&amp;I2</f>
+        <v>sg_ar6_r10</v>
+      </c>
+      <c r="J5" t="str">
+        <f>"sg_"&amp;J2</f>
         <v>sg_timeslice</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" t="str">
-        <f>$A$1&amp;TEXT(N6,"0000")</f>
-        <v>vstacks_t1~0001</v>
+    <row r="6" spans="1:21">
+      <c r="A6">
+        <v>1</v>
       </c>
       <c r="B6" t="str">
-        <f>G6</f>
-        <v>Postponed Transition_3d</v>
-      </c>
-      <c r="G6" t="str">
-        <f>H6&amp;P6</f>
-        <v>Postponed Transition_3d</v>
-      </c>
-      <c r="H6" t="s">
+        <f t="shared" ref="B6:B37" si="0">"vstacks_"&amp;VLOOKUP(A6,$S$6:$T$18,2,FALSE)&amp;"~"&amp;TEXT(O6,"0000")</f>
+        <v>vstacks_s1p1v1_d~0001</v>
+      </c>
+      <c r="C6" t="str">
+        <f>H6</f>
+        <v>e 1.5 deg no OS.e3d</v>
+      </c>
+      <c r="H6" t="str">
+        <f>_xlfn.TEXTJOIN(".",TRUE,I6:J6)</f>
+        <v>e 1.5 deg no OS.e3d</v>
+      </c>
+      <c r="I6" t="s">
+        <v>260</v>
+      </c>
+      <c r="J6" t="str">
+        <f>Q6</f>
+        <v>e3d</v>
+      </c>
+      <c r="L6" t="s">
+        <v>252</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="str">
+        <f>VLOOKUP(A6,$S$6:$U$17,3,FALSE)</f>
+        <v>e3d</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6" t="s">
+        <v>232</v>
+      </c>
+      <c r="U6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s1p1v1_d~0002</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" ref="C7:C26" si="1">H7</f>
+        <v>d 1.5 deg OS.e3d</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" ref="H7:H55" si="2">_xlfn.TEXTJOIN(".",TRUE,I7:J7)</f>
+        <v>d 1.5 deg OS.e3d</v>
+      </c>
+      <c r="I7" t="s">
+        <v>259</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" ref="J7:J55" si="3">Q7</f>
+        <v>e3d</v>
+      </c>
+      <c r="L7" t="s">
+        <v>253</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" ref="Q7:Q55" si="4">VLOOKUP(A7,$S$6:$U$17,3,FALSE)</f>
+        <v>e3d</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="T7" t="s">
+        <v>233</v>
+      </c>
+      <c r="U7" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s1p1v1_d~0003</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>c 2 deg (67%).e3d</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="2"/>
+        <v>c 2 deg (67%).e3d</v>
+      </c>
+      <c r="I8" t="s">
+        <v>258</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="3"/>
+        <v>e3d</v>
+      </c>
+      <c r="L8" t="s">
         <v>254</v>
       </c>
-      <c r="I6" t="s">
-        <v>132</v>
-      </c>
-      <c r="N6">
+      <c r="O8">
+        <v>3</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="4"/>
+        <v>e3d</v>
+      </c>
+      <c r="S8">
+        <v>3</v>
+      </c>
+      <c r="T8" t="s">
+        <v>234</v>
+      </c>
+      <c r="U8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9">
         <v>1</v>
       </c>
-      <c r="P6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" t="str">
-        <f t="shared" ref="A7:A12" si="0">$A$1&amp;TEXT(N7,"0000")</f>
-        <v>vstacks_t1~0002</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" ref="B7:B26" si="1">G7</f>
-        <v>Target Net Zero 2050_3d</v>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" ref="G7:G26" si="2">H7&amp;P7</f>
-        <v>Target Net Zero 2050_3d</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s1p1v1_d~0004</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>b 2 deg (50%).e3d</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="2"/>
+        <v>b 2 deg (50%).e3d</v>
+      </c>
+      <c r="I9" t="s">
+        <v>257</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="3"/>
+        <v>e3d</v>
+      </c>
+      <c r="L9" t="s">
         <v>255</v>
       </c>
-      <c r="I7" t="s">
-        <v>132</v>
-      </c>
-      <c r="N7">
+      <c r="O9">
+        <v>4</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="4"/>
+        <v>e3d</v>
+      </c>
+      <c r="S9">
+        <v>4</v>
+      </c>
+      <c r="T9" t="s">
+        <v>235</v>
+      </c>
+      <c r="U9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s1p1v1_d~0005</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>a 3 deg.e3d</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="2"/>
+        <v>a 3 deg.e3d</v>
+      </c>
+      <c r="I10" t="s">
+        <v>261</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="3"/>
+        <v>e3d</v>
+      </c>
+      <c r="L10" t="s">
+        <v>256</v>
+      </c>
+      <c r="O10">
+        <v>5</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="4"/>
+        <v>e3d</v>
+      </c>
+      <c r="S10">
+        <v>5</v>
+      </c>
+      <c r="T10" t="s">
+        <v>236</v>
+      </c>
+      <c r="U10" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11">
+        <f>A6+1</f>
         <v>2</v>
       </c>
-      <c r="P7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" t="str">
-        <f t="shared" si="0"/>
-        <v>vstacks_t1~0003</v>
-      </c>
-      <c r="B8" t="str">
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s3p3v3_d~0001</v>
+      </c>
+      <c r="C11" t="str">
         <f t="shared" si="1"/>
-        <v>Declared NDCs_3d</v>
-      </c>
-      <c r="G8" t="str">
+        <v>e 1.5 deg no OS.d9d</v>
+      </c>
+      <c r="H11" t="str">
         <f t="shared" si="2"/>
-        <v>Declared NDCs_3d</v>
-      </c>
-      <c r="H8" t="s">
-        <v>252</v>
-      </c>
-      <c r="I8" t="s">
-        <v>132</v>
-      </c>
-      <c r="N8">
+        <v>e 1.5 deg no OS.d9d</v>
+      </c>
+      <c r="I11" t="str">
+        <f>I6</f>
+        <v>e 1.5 deg no OS</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="3"/>
+        <v>d9d</v>
+      </c>
+      <c r="O11">
+        <f>O6</f>
+        <v>1</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="4"/>
+        <v>d9d</v>
+      </c>
+      <c r="S11">
+        <v>6</v>
+      </c>
+      <c r="T11" t="s">
+        <v>237</v>
+      </c>
+      <c r="U11" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12">
+        <f t="shared" ref="A12:A55" si="5">A7+1</f>
+        <v>2</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s3p3v3_d~0002</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1.5 deg OS.d9d</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v>d 1.5 deg OS.d9d</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" ref="I12:I55" si="6">I7</f>
+        <v>d 1.5 deg OS</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="3"/>
+        <v>d9d</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ref="O12:O55" si="7">O7</f>
+        <v>2</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="4"/>
+        <v>d9d</v>
+      </c>
+      <c r="S12">
+        <v>7</v>
+      </c>
+      <c r="T12" t="s">
+        <v>238</v>
+      </c>
+      <c r="U12" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s3p3v3_d~0003</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>c 2 deg (67%).d9d</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="2"/>
+        <v>c 2 deg (67%).d9d</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="6"/>
+        <v>c 2 deg (67%)</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="3"/>
+        <v>d9d</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="P8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" t="str">
-        <f t="shared" si="0"/>
-        <v>vstacks_t1~0004</v>
-      </c>
-      <c r="B9" t="str">
+      <c r="Q13" t="str">
+        <f t="shared" si="4"/>
+        <v>d9d</v>
+      </c>
+      <c r="S13">
+        <v>8</v>
+      </c>
+      <c r="T13" t="s">
+        <v>239</v>
+      </c>
+      <c r="U13" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s3p3v3_d~0004</v>
+      </c>
+      <c r="C14" t="str">
         <f t="shared" si="1"/>
-        <v>Limited to 2 deg_3d</v>
-      </c>
-      <c r="G9" t="str">
+        <v>b 2 deg (50%).d9d</v>
+      </c>
+      <c r="H14" t="str">
         <f t="shared" si="2"/>
-        <v>Limited to 2 deg_3d</v>
-      </c>
-      <c r="H9" t="s">
-        <v>253</v>
-      </c>
-      <c r="I9" t="s">
-        <v>132</v>
-      </c>
-      <c r="N9">
+        <v>b 2 deg (50%).d9d</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="6"/>
+        <v>b 2 deg (50%)</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="3"/>
+        <v>d9d</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="P9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" t="str">
-        <f t="shared" si="0"/>
-        <v>vstacks_t1~0005</v>
-      </c>
-      <c r="B10" t="str">
+      <c r="Q14" t="str">
+        <f t="shared" si="4"/>
+        <v>d9d</v>
+      </c>
+      <c r="S14">
+        <v>9</v>
+      </c>
+      <c r="T14" t="s">
+        <v>241</v>
+      </c>
+      <c r="U14" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s3p3v3_d~0005</v>
+      </c>
+      <c r="C15" t="str">
         <f t="shared" si="1"/>
-        <v>Current Policies_3d</v>
-      </c>
-      <c r="G10" t="str">
+        <v>a 3 deg.d9d</v>
+      </c>
+      <c r="H15" t="str">
         <f t="shared" si="2"/>
-        <v>Current Policies_3d</v>
-      </c>
-      <c r="H10" t="s">
-        <v>256</v>
-      </c>
-      <c r="I10" t="s">
-        <v>132</v>
-      </c>
-      <c r="N10">
+        <v>a 3 deg.d9d</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="6"/>
+        <v>a 3 deg</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="3"/>
+        <v>d9d</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="P10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" t="str">
-        <f t="shared" si="0"/>
-        <v>vstacks_t1~0006</v>
-      </c>
-      <c r="B11" t="str">
-        <f t="shared" si="1"/>
-        <v>Low demand_3d</v>
-      </c>
-      <c r="G11" t="str">
-        <f t="shared" si="2"/>
-        <v>Low demand_3d</v>
-      </c>
-      <c r="H11" t="s">
-        <v>130</v>
-      </c>
-      <c r="I11" t="s">
-        <v>132</v>
-      </c>
-      <c r="N11">
-        <v>6</v>
-      </c>
-      <c r="P11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" t="str">
-        <f t="shared" si="0"/>
-        <v>vstacks_t1~0007</v>
-      </c>
-      <c r="B12" t="str">
-        <f t="shared" si="1"/>
-        <v>Fragmented World_3d</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="2"/>
-        <v>Fragmented World_3d</v>
-      </c>
-      <c r="H12" t="s">
-        <v>131</v>
-      </c>
-      <c r="I12" t="s">
-        <v>132</v>
-      </c>
-      <c r="N12">
-        <v>7</v>
-      </c>
-      <c r="P12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" t="str">
-        <f>$B$1&amp;TEXT(N13,"0000")</f>
-        <v>vstacks_t5~0001</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" si="1"/>
-        <v>Postponed Transition_15d</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" si="2"/>
-        <v>Postponed Transition_15d</v>
-      </c>
-      <c r="H13" t="str">
-        <f>H6</f>
-        <v>Postponed Transition</v>
-      </c>
-      <c r="I13" t="s">
-        <v>133</v>
-      </c>
-      <c r="N13">
-        <f>N6</f>
-        <v>1</v>
-      </c>
-      <c r="P13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" t="str">
-        <f t="shared" ref="A14:A19" si="3">$B$1&amp;TEXT(N14,"0000")</f>
-        <v>vstacks_t5~0002</v>
-      </c>
-      <c r="B14" t="str">
-        <f t="shared" si="1"/>
-        <v>Target Net Zero 2050_15d</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="2"/>
-        <v>Target Net Zero 2050_15d</v>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" ref="H14:H40" si="4">H7</f>
-        <v>Target Net Zero 2050</v>
-      </c>
-      <c r="I14" t="s">
-        <v>133</v>
-      </c>
-      <c r="N14">
-        <f t="shared" ref="N14:N40" si="5">N7</f>
-        <v>2</v>
-      </c>
-      <c r="P14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" t="str">
-        <f t="shared" si="3"/>
-        <v>vstacks_t5~0003</v>
-      </c>
-      <c r="B15" t="str">
-        <f t="shared" si="1"/>
-        <v>Declared NDCs_15d</v>
-      </c>
-      <c r="G15" t="str">
-        <f t="shared" si="2"/>
-        <v>Declared NDCs_15d</v>
-      </c>
-      <c r="H15" t="str">
+      <c r="Q15" t="str">
         <f t="shared" si="4"/>
-        <v>Declared NDCs</v>
-      </c>
-      <c r="I15" t="s">
-        <v>133</v>
-      </c>
-      <c r="N15">
+        <v>d9d</v>
+      </c>
+      <c r="S15">
+        <v>10</v>
+      </c>
+      <c r="T15" t="s">
+        <v>240</v>
+      </c>
+      <c r="U15" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="P15" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" t="str">
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s2_w~0001</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>e 1.5 deg no OS.b2w</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="2"/>
+        <v>e 1.5 deg no OS.b2w</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="6"/>
+        <v>e 1.5 deg no OS</v>
+      </c>
+      <c r="J16" t="str">
         <f t="shared" si="3"/>
-        <v>vstacks_t5~0004</v>
-      </c>
-      <c r="B16" t="str">
+        <v>b2w</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q16" t="str">
+        <f t="shared" si="4"/>
+        <v>b2w</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s2_w~0002</v>
+      </c>
+      <c r="C17" t="str">
         <f t="shared" si="1"/>
-        <v>Limited to 2 deg_15d</v>
-      </c>
-      <c r="G16" t="str">
+        <v>d 1.5 deg OS.b2w</v>
+      </c>
+      <c r="H17" t="str">
         <f t="shared" si="2"/>
-        <v>Limited to 2 deg_15d</v>
-      </c>
-      <c r="H16" t="str">
+        <v>d 1.5 deg OS.b2w</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="6"/>
+        <v>d 1.5 deg OS</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="3"/>
+        <v>b2w</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="Q17" t="str">
         <f t="shared" si="4"/>
-        <v>Limited to 2 deg</v>
-      </c>
-      <c r="I16" t="s">
-        <v>133</v>
-      </c>
-      <c r="N16">
+        <v>b2w</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s2_w~0003</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="1"/>
+        <v>c 2 deg (67%).b2w</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="2"/>
+        <v>c 2 deg (67%).b2w</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="6"/>
+        <v>c 2 deg (67%)</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="3"/>
+        <v>b2w</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="4"/>
+        <v>b2w</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s2_w~0004</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>b 2 deg (50%).b2w</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="2"/>
+        <v>b 2 deg (50%).b2w</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="6"/>
+        <v>b 2 deg (50%)</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="3"/>
+        <v>b2w</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="4"/>
+        <v>b2w</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s2_w~0005</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>a 3 deg.b2w</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="2"/>
+        <v>a 3 deg.b2w</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="6"/>
+        <v>a 3 deg</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="3"/>
+        <v>b2w</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" si="4"/>
+        <v>b2w</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="P16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
-      <c r="A17" t="str">
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s2_w_p2_d~0001</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>e 1.5 deg no OS.a2w2d</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="2"/>
+        <v>e 1.5 deg no OS.a2w2d</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="6"/>
+        <v>e 1.5 deg no OS</v>
+      </c>
+      <c r="J21" t="str">
         <f t="shared" si="3"/>
-        <v>vstacks_t5~0005</v>
-      </c>
-      <c r="B17" t="str">
+        <v>a2w2d</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="4"/>
+        <v>a2w2d</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s2_w_p2_d~0002</v>
+      </c>
+      <c r="C22" t="str">
         <f t="shared" si="1"/>
-        <v>Current Policies_15d</v>
-      </c>
-      <c r="G17" t="str">
+        <v>d 1.5 deg OS.a2w2d</v>
+      </c>
+      <c r="H22" t="str">
         <f t="shared" si="2"/>
-        <v>Current Policies_15d</v>
-      </c>
-      <c r="H17" t="str">
+        <v>d 1.5 deg OS.a2w2d</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="6"/>
+        <v>d 1.5 deg OS</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="3"/>
+        <v>a2w2d</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="Q22" t="str">
         <f t="shared" si="4"/>
-        <v>Current Policies</v>
-      </c>
-      <c r="I17" t="s">
-        <v>133</v>
-      </c>
-      <c r="N17">
+        <v>a2w2d</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s2_w_p2_d~0003</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="1"/>
+        <v>c 2 deg (67%).a2w2d</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="2"/>
+        <v>c 2 deg (67%).a2w2d</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="6"/>
+        <v>c 2 deg (67%)</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="3"/>
+        <v>a2w2d</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="Q23" t="str">
+        <f t="shared" si="4"/>
+        <v>a2w2d</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s2_w_p2_d~0004</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v>b 2 deg (50%).a2w2d</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="2"/>
+        <v>b 2 deg (50%).a2w2d</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="6"/>
+        <v>b 2 deg (50%)</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="3"/>
+        <v>a2w2d</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="Q24" t="str">
+        <f t="shared" si="4"/>
+        <v>a2w2d</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_s2_w_p2_d~0005</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="1"/>
+        <v>a 3 deg.a2w2d</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="2"/>
+        <v>a 3 deg.a2w2d</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="6"/>
+        <v>a 3 deg</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="3"/>
+        <v>a2w2d</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="Q25" t="str">
+        <f t="shared" si="4"/>
+        <v>a2w2d</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="P17" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
-      <c r="A18" t="str">
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_ts12_clu~0001</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="1"/>
+        <v>e 1.5 deg no OS.hTS12c</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="2"/>
+        <v>e 1.5 deg no OS.hTS12c</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="6"/>
+        <v>e 1.5 deg no OS</v>
+      </c>
+      <c r="J26" t="str">
         <f t="shared" si="3"/>
-        <v>vstacks_t5~0006</v>
-      </c>
-      <c r="B18" t="str">
-        <f t="shared" si="1"/>
-        <v>Low demand_15d</v>
-      </c>
-      <c r="G18" t="str">
+        <v>hTS12c</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q26" t="str">
+        <f t="shared" si="4"/>
+        <v>hTS12c</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_ts12_clu~0002</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" ref="C27:C40" si="8">H27</f>
+        <v>d 1.5 deg OS.hTS12c</v>
+      </c>
+      <c r="H27" t="str">
         <f t="shared" si="2"/>
-        <v>Low demand_15d</v>
-      </c>
-      <c r="H18" t="str">
+        <v>d 1.5 deg OS.hTS12c</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="6"/>
+        <v>d 1.5 deg OS</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="3"/>
+        <v>hTS12c</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="Q27" t="str">
         <f t="shared" si="4"/>
-        <v>Low demand</v>
-      </c>
-      <c r="I18" t="s">
-        <v>133</v>
-      </c>
-      <c r="N18">
+        <v>hTS12c</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_ts12_clu~0003</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="8"/>
+        <v>c 2 deg (67%).hTS12c</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="2"/>
+        <v>c 2 deg (67%).hTS12c</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="6"/>
+        <v>c 2 deg (67%)</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="3"/>
+        <v>hTS12c</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="Q28" t="str">
+        <f t="shared" si="4"/>
+        <v>hTS12c</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_ts12_clu~0004</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="8"/>
+        <v>b 2 deg (50%).hTS12c</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="2"/>
+        <v>b 2 deg (50%).hTS12c</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="6"/>
+        <v>b 2 deg (50%)</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="3"/>
+        <v>hTS12c</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="Q29" t="str">
+        <f t="shared" si="4"/>
+        <v>hTS12c</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_ts12_clu~0005</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="8"/>
+        <v>a 3 deg.hTS12c</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="2"/>
+        <v>a 3 deg.hTS12c</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="6"/>
+        <v>a 3 deg</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="3"/>
+        <v>hTS12c</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="Q30" t="str">
+        <f t="shared" si="4"/>
+        <v>hTS12c</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="P18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="A19" t="str">
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_ts24_clu~0001</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="8"/>
+        <v>e 1.5 deg no OS.gTS24c</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="2"/>
+        <v>e 1.5 deg no OS.gTS24c</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="6"/>
+        <v>e 1.5 deg no OS</v>
+      </c>
+      <c r="J31" t="str">
         <f t="shared" si="3"/>
-        <v>vstacks_t5~0007</v>
-      </c>
-      <c r="B19" t="str">
-        <f t="shared" si="1"/>
-        <v>Fragmented World_15d</v>
-      </c>
-      <c r="G19" t="str">
+        <v>gTS24c</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q31" t="str">
+        <f t="shared" si="4"/>
+        <v>gTS24c</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_ts24_clu~0002</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="8"/>
+        <v>d 1.5 deg OS.gTS24c</v>
+      </c>
+      <c r="H32" t="str">
         <f t="shared" si="2"/>
-        <v>Fragmented World_15d</v>
-      </c>
-      <c r="H19" t="str">
+        <v>d 1.5 deg OS.gTS24c</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="6"/>
+        <v>d 1.5 deg OS</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="3"/>
+        <v>gTS24c</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="Q32" t="str">
         <f t="shared" si="4"/>
-        <v>Fragmented World</v>
-      </c>
-      <c r="I19" t="s">
-        <v>133</v>
-      </c>
-      <c r="N19">
+        <v>gTS24c</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_ts24_clu~0003</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="8"/>
+        <v>c 2 deg (67%).gTS24c</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="2"/>
+        <v>c 2 deg (67%).gTS24c</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="6"/>
+        <v>c 2 deg (67%)</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="3"/>
+        <v>gTS24c</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="Q33" t="str">
+        <f t="shared" si="4"/>
+        <v>gTS24c</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_ts24_clu~0004</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="8"/>
+        <v>b 2 deg (50%).gTS24c</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="2"/>
+        <v>b 2 deg (50%).gTS24c</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="6"/>
+        <v>b 2 deg (50%)</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="3"/>
+        <v>gTS24c</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" si="4"/>
+        <v>gTS24c</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_ts24_clu~0005</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="8"/>
+        <v>a 3 deg.gTS24c</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="2"/>
+        <v>a 3 deg.gTS24c</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="6"/>
+        <v>a 3 deg</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="3"/>
+        <v>gTS24c</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="Q35" t="str">
+        <f t="shared" si="4"/>
+        <v>gTS24c</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="P19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16">
-      <c r="A20" t="str">
-        <f>$C$1&amp;TEXT(N20,"0000")</f>
-        <v>vstacks_w2~0001</v>
-      </c>
-      <c r="B20" t="str">
-        <f t="shared" si="1"/>
-        <v>Postponed Transition_2w</v>
-      </c>
-      <c r="G20" t="str">
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_ts48_clu~0001</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="8"/>
+        <v>e 1.5 deg no OS.fTS48c</v>
+      </c>
+      <c r="H36" t="str">
         <f t="shared" si="2"/>
-        <v>Postponed Transition_2w</v>
-      </c>
-      <c r="H20" t="str">
+        <v>e 1.5 deg no OS.fTS48c</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="6"/>
+        <v>e 1.5 deg no OS</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="3"/>
+        <v>fTS48c</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q36" t="str">
         <f t="shared" si="4"/>
-        <v>Postponed Transition</v>
-      </c>
-      <c r="I20" t="s">
-        <v>134</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="P20" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16">
-      <c r="A21" t="str">
-        <f t="shared" ref="A21:A26" si="6">$C$1&amp;TEXT(N21,"0000")</f>
-        <v>vstacks_w2~0002</v>
-      </c>
-      <c r="B21" t="str">
-        <f t="shared" si="1"/>
-        <v>Target Net Zero 2050_2w</v>
-      </c>
-      <c r="G21" t="str">
-        <f t="shared" si="2"/>
-        <v>Target Net Zero 2050_2w</v>
-      </c>
-      <c r="H21" t="str">
-        <f t="shared" si="4"/>
-        <v>Target Net Zero 2050</v>
-      </c>
-      <c r="I21" t="s">
-        <v>134</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="P21" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
-      <c r="A22" t="str">
-        <f t="shared" si="6"/>
-        <v>vstacks_w2~0003</v>
-      </c>
-      <c r="B22" t="str">
-        <f t="shared" si="1"/>
-        <v>Declared NDCs_2w</v>
-      </c>
-      <c r="G22" t="str">
-        <f t="shared" si="2"/>
-        <v>Declared NDCs_2w</v>
-      </c>
-      <c r="H22" t="str">
-        <f t="shared" si="4"/>
-        <v>Declared NDCs</v>
-      </c>
-      <c r="I22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N22">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="P22" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="A23" t="str">
-        <f t="shared" si="6"/>
-        <v>vstacks_w2~0004</v>
-      </c>
-      <c r="B23" t="str">
-        <f t="shared" si="1"/>
-        <v>Limited to 2 deg_2w</v>
-      </c>
-      <c r="G23" t="str">
-        <f t="shared" si="2"/>
-        <v>Limited to 2 deg_2w</v>
-      </c>
-      <c r="H23" t="str">
-        <f t="shared" si="4"/>
-        <v>Limited to 2 deg</v>
-      </c>
-      <c r="I23" t="s">
-        <v>134</v>
-      </c>
-      <c r="N23">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="P23" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
-      <c r="A24" t="str">
-        <f t="shared" si="6"/>
-        <v>vstacks_w2~0005</v>
-      </c>
-      <c r="B24" t="str">
-        <f t="shared" si="1"/>
-        <v>Current Policies_2w</v>
-      </c>
-      <c r="G24" t="str">
-        <f t="shared" si="2"/>
-        <v>Current Policies_2w</v>
-      </c>
-      <c r="H24" t="str">
-        <f t="shared" si="4"/>
-        <v>Current Policies</v>
-      </c>
-      <c r="I24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N24">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P24" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
-      <c r="A25" t="str">
-        <f t="shared" si="6"/>
-        <v>vstacks_w2~0006</v>
-      </c>
-      <c r="B25" t="str">
-        <f t="shared" si="1"/>
-        <v>Low demand_2w</v>
-      </c>
-      <c r="G25" t="str">
-        <f t="shared" si="2"/>
-        <v>Low demand_2w</v>
-      </c>
-      <c r="H25" t="str">
-        <f t="shared" si="4"/>
-        <v>Low demand</v>
-      </c>
-      <c r="I25" t="s">
-        <v>134</v>
-      </c>
-      <c r="N25">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="P25" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="A26" t="str">
-        <f t="shared" si="6"/>
-        <v>vstacks_w2~0007</v>
-      </c>
-      <c r="B26" t="str">
-        <f t="shared" si="1"/>
-        <v>Fragmented World_2w</v>
-      </c>
-      <c r="G26" t="str">
-        <f t="shared" si="2"/>
-        <v>Fragmented World_2w</v>
-      </c>
-      <c r="H26" t="str">
-        <f t="shared" si="4"/>
-        <v>Fragmented World</v>
-      </c>
-      <c r="I26" t="s">
-        <v>134</v>
-      </c>
-      <c r="N26">
+        <v>fTS48c</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="P26" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
-      <c r="A27" t="str">
-        <f>$D$1&amp;TEXT(N27,"0000")</f>
-        <v>vstacks_ts16~0001</v>
-      </c>
-      <c r="B27" t="str">
-        <f t="shared" ref="B27:B40" si="7">G27</f>
-        <v>Postponed Transition_16</v>
-      </c>
-      <c r="G27" t="str">
-        <f t="shared" ref="G27:G40" si="8">H27&amp;P27</f>
-        <v>Postponed Transition_16</v>
-      </c>
-      <c r="H27" t="str">
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>vstacks_ts48_clu~0002</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="8"/>
+        <v>d 1.5 deg OS.fTS48c</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="2"/>
+        <v>d 1.5 deg OS.fTS48c</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="6"/>
+        <v>d 1.5 deg OS</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="3"/>
+        <v>fTS48c</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="Q37" t="str">
         <f t="shared" si="4"/>
-        <v>Postponed Transition</v>
-      </c>
-      <c r="I27" t="s">
-        <v>173</v>
-      </c>
-      <c r="N27">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="P27" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16">
-      <c r="A28" t="str">
-        <f t="shared" ref="A28:A33" si="9">$D$1&amp;TEXT(N28,"0000")</f>
-        <v>vstacks_ts16~0002</v>
-      </c>
-      <c r="B28" t="str">
-        <f t="shared" si="7"/>
-        <v>Target Net Zero 2050_16</v>
-      </c>
-      <c r="G28" t="str">
-        <f t="shared" si="8"/>
-        <v>Target Net Zero 2050_16</v>
-      </c>
-      <c r="H28" t="str">
-        <f t="shared" si="4"/>
-        <v>Target Net Zero 2050</v>
-      </c>
-      <c r="I28" t="s">
-        <v>173</v>
-      </c>
-      <c r="N28">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="P28" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
-      <c r="A29" t="str">
-        <f t="shared" si="9"/>
-        <v>vstacks_ts16~0003</v>
-      </c>
-      <c r="B29" t="str">
-        <f t="shared" si="7"/>
-        <v>Declared NDCs_16</v>
-      </c>
-      <c r="G29" t="str">
-        <f t="shared" si="8"/>
-        <v>Declared NDCs_16</v>
-      </c>
-      <c r="H29" t="str">
-        <f t="shared" si="4"/>
-        <v>Declared NDCs</v>
-      </c>
-      <c r="I29" t="s">
-        <v>173</v>
-      </c>
-      <c r="N29">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="P29" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16">
-      <c r="A30" t="str">
-        <f t="shared" si="9"/>
-        <v>vstacks_ts16~0004</v>
-      </c>
-      <c r="B30" t="str">
-        <f t="shared" si="7"/>
-        <v>Limited to 2 deg_16</v>
-      </c>
-      <c r="G30" t="str">
-        <f t="shared" si="8"/>
-        <v>Limited to 2 deg_16</v>
-      </c>
-      <c r="H30" t="str">
-        <f t="shared" si="4"/>
-        <v>Limited to 2 deg</v>
-      </c>
-      <c r="I30" t="s">
-        <v>173</v>
-      </c>
-      <c r="N30">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="P30" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16">
-      <c r="A31" t="str">
-        <f t="shared" si="9"/>
-        <v>vstacks_ts16~0005</v>
-      </c>
-      <c r="B31" t="str">
-        <f t="shared" si="7"/>
-        <v>Current Policies_16</v>
-      </c>
-      <c r="G31" t="str">
-        <f t="shared" si="8"/>
-        <v>Current Policies_16</v>
-      </c>
-      <c r="H31" t="str">
-        <f t="shared" si="4"/>
-        <v>Current Policies</v>
-      </c>
-      <c r="I31" t="s">
-        <v>173</v>
-      </c>
-      <c r="N31">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P31" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16">
-      <c r="A32" t="str">
-        <f t="shared" si="9"/>
-        <v>vstacks_ts16~0006</v>
-      </c>
-      <c r="B32" t="str">
-        <f t="shared" si="7"/>
-        <v>Low demand_16</v>
-      </c>
-      <c r="G32" t="str">
-        <f t="shared" si="8"/>
-        <v>Low demand_16</v>
-      </c>
-      <c r="H32" t="str">
-        <f t="shared" si="4"/>
-        <v>Low demand</v>
-      </c>
-      <c r="I32" t="s">
-        <v>173</v>
-      </c>
-      <c r="N32">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="P32" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16">
-      <c r="A33" t="str">
-        <f t="shared" si="9"/>
-        <v>vstacks_ts16~0007</v>
-      </c>
-      <c r="B33" t="str">
-        <f t="shared" si="7"/>
-        <v>Fragmented World_16</v>
-      </c>
-      <c r="G33" t="str">
-        <f t="shared" si="8"/>
-        <v>Fragmented World_16</v>
-      </c>
-      <c r="H33" t="str">
-        <f t="shared" si="4"/>
-        <v>Fragmented World</v>
-      </c>
-      <c r="I33" t="s">
-        <v>173</v>
-      </c>
-      <c r="N33">
+        <v>fTS48c</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="P33" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16">
-      <c r="A34" t="str">
-        <f>$E$1&amp;TEXT(N34,"0000")</f>
-        <v>vstacks_t_annual~0001</v>
-      </c>
-      <c r="B34" t="str">
+      <c r="B38" t="str">
+        <f t="shared" ref="B38:B55" si="9">"vstacks_"&amp;VLOOKUP(A38,$S$6:$T$18,2,FALSE)&amp;"~"&amp;TEXT(O38,"0000")</f>
+        <v>vstacks_ts48_clu~0003</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="8"/>
+        <v>c 2 deg (67%).fTS48c</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="2"/>
+        <v>c 2 deg (67%).fTS48c</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="6"/>
+        <v>c 2 deg (67%)</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="3"/>
+        <v>fTS48c</v>
+      </c>
+      <c r="O38">
         <f t="shared" si="7"/>
-        <v>Postponed Transition_ann</v>
-      </c>
-      <c r="G34" t="str">
-        <f t="shared" si="8"/>
-        <v>Postponed Transition_ann</v>
-      </c>
-      <c r="H34" t="str">
+        <v>3</v>
+      </c>
+      <c r="Q38" t="str">
         <f t="shared" si="4"/>
-        <v>Postponed Transition</v>
-      </c>
-      <c r="I34" t="s">
-        <v>174</v>
-      </c>
-      <c r="N34">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="P34" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16">
-      <c r="A35" t="str">
-        <f t="shared" ref="A35:A40" si="10">$E$1&amp;TEXT(N35,"0000")</f>
-        <v>vstacks_t_annual~0002</v>
-      </c>
-      <c r="B35" t="str">
-        <f t="shared" si="7"/>
-        <v>Target Net Zero 2050_ann</v>
-      </c>
-      <c r="G35" t="str">
-        <f t="shared" si="8"/>
-        <v>Target Net Zero 2050_ann</v>
-      </c>
-      <c r="H35" t="str">
-        <f t="shared" si="4"/>
-        <v>Target Net Zero 2050</v>
-      </c>
-      <c r="I35" t="s">
-        <v>174</v>
-      </c>
-      <c r="N35">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="P35" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16">
-      <c r="A36" t="str">
-        <f t="shared" si="10"/>
-        <v>vstacks_t_annual~0003</v>
-      </c>
-      <c r="B36" t="str">
-        <f t="shared" si="7"/>
-        <v>Declared NDCs_ann</v>
-      </c>
-      <c r="G36" t="str">
-        <f t="shared" si="8"/>
-        <v>Declared NDCs_ann</v>
-      </c>
-      <c r="H36" t="str">
-        <f t="shared" si="4"/>
-        <v>Declared NDCs</v>
-      </c>
-      <c r="I36" t="s">
-        <v>174</v>
-      </c>
-      <c r="N36">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="P36" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16">
-      <c r="A37" t="str">
-        <f t="shared" si="10"/>
-        <v>vstacks_t_annual~0004</v>
-      </c>
-      <c r="B37" t="str">
-        <f t="shared" si="7"/>
-        <v>Limited to 2 deg_ann</v>
-      </c>
-      <c r="G37" t="str">
-        <f t="shared" si="8"/>
-        <v>Limited to 2 deg_ann</v>
-      </c>
-      <c r="H37" t="str">
-        <f t="shared" si="4"/>
-        <v>Limited to 2 deg</v>
-      </c>
-      <c r="I37" t="s">
-        <v>174</v>
-      </c>
-      <c r="N37">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="P37" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16">
-      <c r="A38" t="str">
-        <f t="shared" si="10"/>
-        <v>vstacks_t_annual~0005</v>
-      </c>
-      <c r="B38" t="str">
-        <f t="shared" si="7"/>
-        <v>Current Policies_ann</v>
-      </c>
-      <c r="G38" t="str">
-        <f t="shared" si="8"/>
-        <v>Current Policies_ann</v>
-      </c>
-      <c r="H38" t="str">
-        <f t="shared" si="4"/>
-        <v>Current Policies</v>
-      </c>
-      <c r="I38" t="s">
-        <v>174</v>
-      </c>
-      <c r="N38">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="P38" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16">
-      <c r="A39" t="str">
-        <f t="shared" si="10"/>
-        <v>vstacks_t_annual~0006</v>
-      </c>
-      <c r="B39" t="str">
-        <f t="shared" si="7"/>
-        <v>Low demand_ann</v>
-      </c>
-      <c r="G39" t="str">
-        <f t="shared" si="8"/>
-        <v>Low demand_ann</v>
-      </c>
-      <c r="H39" t="str">
-        <f t="shared" si="4"/>
-        <v>Low demand</v>
-      </c>
-      <c r="I39" t="s">
-        <v>174</v>
-      </c>
-      <c r="N39">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="P39" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16">
-      <c r="A40" t="str">
-        <f t="shared" si="10"/>
-        <v>vstacks_t_annual~0007</v>
-      </c>
-      <c r="B40" t="str">
-        <f t="shared" si="7"/>
-        <v>Fragmented World_ann</v>
-      </c>
-      <c r="G40" t="str">
-        <f t="shared" si="8"/>
-        <v>Fragmented World_ann</v>
-      </c>
-      <c r="H40" t="str">
-        <f t="shared" si="4"/>
-        <v>Fragmented World</v>
-      </c>
-      <c r="I40" t="s">
-        <v>174</v>
-      </c>
-      <c r="N40">
+        <v>fTS48c</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="P40" t="s">
-        <v>176</v>
+      <c r="B39" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts48_clu~0004</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="8"/>
+        <v>b 2 deg (50%).fTS48c</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="2"/>
+        <v>b 2 deg (50%).fTS48c</v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="6"/>
+        <v>b 2 deg (50%)</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="3"/>
+        <v>fTS48c</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="Q39" t="str">
+        <f t="shared" si="4"/>
+        <v>fTS48c</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts48_clu~0005</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="8"/>
+        <v>a 3 deg.fTS48c</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="2"/>
+        <v>a 3 deg.fTS48c</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="6"/>
+        <v>a 3 deg</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="3"/>
+        <v>fTS48c</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="Q40" t="str">
+        <f t="shared" si="4"/>
+        <v>fTS48c</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_s5p5v5_d~0001</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" ref="C41:C55" si="10">H41</f>
+        <v>e 1.5 deg no OS.c15d</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="2"/>
+        <v>e 1.5 deg no OS.c15d</v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="6"/>
+        <v>e 1.5 deg no OS</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="3"/>
+        <v>c15d</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q41" t="str">
+        <f t="shared" si="4"/>
+        <v>c15d</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="A42">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_s5p5v5_d~0002</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="10"/>
+        <v>d 1.5 deg OS.c15d</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="2"/>
+        <v>d 1.5 deg OS.c15d</v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="6"/>
+        <v>d 1.5 deg OS</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="3"/>
+        <v>c15d</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="Q42" t="str">
+        <f t="shared" si="4"/>
+        <v>c15d</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_s5p5v5_d~0003</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="10"/>
+        <v>c 2 deg (67%).c15d</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="2"/>
+        <v>c 2 deg (67%).c15d</v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="6"/>
+        <v>c 2 deg (67%)</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="3"/>
+        <v>c15d</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="Q43" t="str">
+        <f t="shared" si="4"/>
+        <v>c15d</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="A44">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_s5p5v5_d~0004</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="10"/>
+        <v>b 2 deg (50%).c15d</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="2"/>
+        <v>b 2 deg (50%).c15d</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" si="6"/>
+        <v>b 2 deg (50%)</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="3"/>
+        <v>c15d</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="Q44" t="str">
+        <f t="shared" si="4"/>
+        <v>c15d</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="A45">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_s5p5v5_d~0005</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="10"/>
+        <v>a 3 deg.c15d</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="2"/>
+        <v>a 3 deg.c15d</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="6"/>
+        <v>a 3 deg</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="3"/>
+        <v>c15d</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="Q45" t="str">
+        <f t="shared" si="4"/>
+        <v>c15d</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
+      <c r="A46">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts_12~0001</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="10"/>
+        <v>e 1.5 deg no OS.iTS12</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="2"/>
+        <v>e 1.5 deg no OS.iTS12</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="6"/>
+        <v>e 1.5 deg no OS</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="3"/>
+        <v>iTS12</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q46" t="str">
+        <f t="shared" si="4"/>
+        <v>iTS12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="A47">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts_12~0002</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="10"/>
+        <v>d 1.5 deg OS.iTS12</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="2"/>
+        <v>d 1.5 deg OS.iTS12</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="6"/>
+        <v>d 1.5 deg OS</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="3"/>
+        <v>iTS12</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="Q47" t="str">
+        <f t="shared" si="4"/>
+        <v>iTS12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
+      <c r="A48">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts_12~0003</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="10"/>
+        <v>c 2 deg (67%).iTS12</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="2"/>
+        <v>c 2 deg (67%).iTS12</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="6"/>
+        <v>c 2 deg (67%)</v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" si="3"/>
+        <v>iTS12</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="Q48" t="str">
+        <f t="shared" si="4"/>
+        <v>iTS12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17">
+      <c r="A49">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts_12~0004</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="10"/>
+        <v>b 2 deg (50%).iTS12</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="2"/>
+        <v>b 2 deg (50%).iTS12</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="6"/>
+        <v>b 2 deg (50%)</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="3"/>
+        <v>iTS12</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="Q49" t="str">
+        <f t="shared" si="4"/>
+        <v>iTS12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17">
+      <c r="A50">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts_12~0005</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="10"/>
+        <v>a 3 deg.iTS12</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="2"/>
+        <v>a 3 deg.iTS12</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="6"/>
+        <v>a 3 deg</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="3"/>
+        <v>iTS12</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="Q50" t="str">
+        <f t="shared" si="4"/>
+        <v>iTS12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17">
+      <c r="A51">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts_annual~0001</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="10"/>
+        <v>e 1.5 deg no OS.jAnn</v>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" si="2"/>
+        <v>e 1.5 deg no OS.jAnn</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="6"/>
+        <v>e 1.5 deg no OS</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="3"/>
+        <v>jAnn</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q51" t="str">
+        <f t="shared" si="4"/>
+        <v>jAnn</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17">
+      <c r="A52">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts_annual~0002</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="10"/>
+        <v>d 1.5 deg OS.jAnn</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="2"/>
+        <v>d 1.5 deg OS.jAnn</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="6"/>
+        <v>d 1.5 deg OS</v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="3"/>
+        <v>jAnn</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="Q52" t="str">
+        <f t="shared" si="4"/>
+        <v>jAnn</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
+      <c r="A53">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="B53" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts_annual~0003</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="10"/>
+        <v>c 2 deg (67%).jAnn</v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="2"/>
+        <v>c 2 deg (67%).jAnn</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="6"/>
+        <v>c 2 deg (67%)</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="3"/>
+        <v>jAnn</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="Q53" t="str">
+        <f t="shared" si="4"/>
+        <v>jAnn</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17">
+      <c r="A54">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="B54" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts_annual~0004</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="10"/>
+        <v>b 2 deg (50%).jAnn</v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="2"/>
+        <v>b 2 deg (50%).jAnn</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="6"/>
+        <v>b 2 deg (50%)</v>
+      </c>
+      <c r="J54" t="str">
+        <f t="shared" si="3"/>
+        <v>jAnn</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="Q54" t="str">
+        <f t="shared" si="4"/>
+        <v>jAnn</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17">
+      <c r="A55">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="9"/>
+        <v>vstacks_ts_annual~0005</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="10"/>
+        <v>a 3 deg.jAnn</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="2"/>
+        <v>a 3 deg.jAnn</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="6"/>
+        <v>a 3 deg</v>
+      </c>
+      <c r="J55" t="str">
+        <f t="shared" si="3"/>
+        <v>jAnn</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="Q55" t="str">
+        <f t="shared" si="4"/>
+        <v>jAnn</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D59:D68">
+    <sortCondition ref="D59:D68"/>
+  </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2627,10 +3466,10 @@
         <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="D5">
         <v>1E-3</v>
@@ -2641,10 +3480,10 @@
         <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="D6">
         <v>-1E-3</v>
@@ -2655,10 +3494,10 @@
         <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D7">
         <v>-1000</v>
@@ -2676,7 +3515,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -2774,7 +3613,7 @@
         <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="K3" t="s">
         <v>8</v>
@@ -2791,7 +3630,7 @@
         <v>116</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="K4" t="s">
         <v>8</v>
@@ -2812,10 +3651,10 @@
         <v>117</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="I5" t="s">
-        <v>178</v>
+        <v>263</v>
       </c>
       <c r="K5" t="s">
         <v>81</v>
@@ -2835,7 +3674,7 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="D6" s="2"/>
       <c r="H6" t="s">
@@ -2861,13 +3700,13 @@
         <v>5</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="K7" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="N7" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
@@ -2877,13 +3716,13 @@
         <v>5</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="K8" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="N8" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
@@ -2936,13 +3775,13 @@
         <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="K11" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="N11" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -3106,7 +3945,7 @@
   <sheetData>
     <row r="3" spans="1:19" ht="17.25" thickBot="1">
       <c r="A3" s="5" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15" thickTop="1" thickBot="1">
@@ -3162,10 +4001,10 @@
         <v>107</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -3181,10 +4020,10 @@
         <v>Elec-220V,Elec-400V,Elec-380V,Elec-225V,Elec-330V,Elec-275V,Elec-420V,Elec-300V,Elec-500V,Elec-750V,Elec-450V,Elec-515V,Elec-525V,Elec-320V,Elec-150V,Elec-270V,Elec-350V,Elec-250V,Elec-200V,Elec-236V,Elec-600V,Solar elec,Wind elec,fossil,renewable,bioenergy,hydrogen,nuclear,ELC,buildings,industry,transport,EVs</v>
       </c>
       <c r="J5" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="M5" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="S5">
         <v>-1</v>
@@ -3192,7 +4031,7 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="B6" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,PSet_MAP!$A$3:$A$49)</f>
@@ -3203,10 +4042,10 @@
         <v>Elec-220V,Elec-400V,Elec-380V,Elec-225V,Elec-330V,Elec-275V,Elec-420V,Elec-300V,Elec-500V,Elec-750V,Elec-450V,Elec-515V,Elec-525V,Elec-320V,Elec-150V,Elec-270V,Elec-350V,Elec-250V,Elec-200V,Elec-236V,Elec-600V,Solar elec,Wind elec,fossil,renewable,bioenergy,hydrogen,nuclear,ELC,buildings,industry,transport,EVs</v>
       </c>
       <c r="J6" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="M6" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="S6">
         <v>-1</v>
@@ -3314,7 +4153,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -3323,7 +4162,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -3350,7 +4189,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -3359,7 +4198,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -3368,7 +4207,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -3377,7 +4216,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
@@ -3386,7 +4225,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -3422,7 +4261,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
@@ -3431,7 +4270,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
@@ -3440,7 +4279,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
@@ -3449,7 +4288,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
@@ -3458,7 +4297,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
@@ -3467,7 +4306,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
@@ -3476,7 +4315,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
@@ -3485,7 +4324,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
@@ -3494,7 +4333,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
@@ -3503,7 +4342,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
@@ -3512,7 +4351,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
@@ -3521,7 +4360,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
@@ -3530,7 +4369,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
@@ -3539,7 +4378,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
@@ -3548,7 +4387,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
@@ -3557,7 +4396,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
@@ -3566,7 +4405,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
@@ -3575,7 +4414,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
@@ -3584,7 +4423,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
@@ -3593,7 +4432,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
@@ -3602,7 +4441,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
@@ -3611,7 +4450,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
@@ -3620,7 +4459,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
@@ -3629,7 +4468,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
@@ -3638,7 +4477,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
@@ -3647,7 +4486,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
@@ -3691,7 +4530,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="B3" t="str">
         <f>A3</f>
@@ -3700,7 +4539,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" ref="B4:B35" si="0">A4</f>
@@ -3709,7 +4548,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
@@ -3718,7 +4557,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -3727,7 +4566,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
@@ -3736,7 +4575,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
@@ -3745,7 +4584,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
@@ -3754,7 +4593,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -3763,7 +4602,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -3772,7 +4611,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
@@ -3781,7 +4620,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
@@ -3790,7 +4629,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -3799,7 +4638,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -3808,7 +4647,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -3817,7 +4656,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
@@ -3826,7 +4665,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -3835,7 +4674,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
@@ -3844,7 +4683,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
@@ -3853,7 +4692,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
@@ -3862,7 +4701,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
@@ -3871,7 +4710,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
@@ -3880,7 +4719,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
@@ -3889,7 +4728,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
@@ -3898,7 +4737,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
@@ -3907,7 +4746,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
@@ -3916,7 +4755,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
@@ -3925,7 +4764,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
@@ -3934,7 +4773,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
@@ -3943,7 +4782,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
@@ -3952,7 +4791,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
@@ -3961,7 +4800,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
@@ -3970,7 +4809,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
@@ -3979,7 +4818,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
@@ -4049,7 +4888,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4065,32 +4904,32 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="C5" t="str">
         <f>LEFT(B5,2)</f>
@@ -4099,10 +4938,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ref="C6:C10" si="0">LEFT(B6,2)</f>
@@ -4111,10 +4950,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -4123,10 +4962,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -4135,10 +4974,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -4147,10 +4986,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -4166,8 +5005,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10ADB714-E6AA-4E3E-B77B-62B65BA0E218}">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4323,7 +5163,7 @@
         <v>Bio Power</v>
       </c>
       <c r="D12" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -4335,7 +5175,7 @@
         <v>Solar Util</v>
       </c>
       <c r="D13" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4371,7 +5211,7 @@
         <v>Geothermal P</v>
       </c>
       <c r="D16" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4383,7 +5223,7 @@
         <v>Hydro Dam</v>
       </c>
       <c r="D17" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -4395,7 +5235,7 @@
         <v>Hydro RoR</v>
       </c>
       <c r="D18" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -4407,7 +5247,7 @@
         <v>Nuclear P</v>
       </c>
       <c r="D19" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4419,7 +5259,7 @@
         <v>Nuclear SMR</v>
       </c>
       <c r="D20" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -4467,7 +5307,7 @@
         <v>Demand</v>
       </c>
       <c r="D24" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -4479,7 +5319,7 @@
         <v>Transformers Dn</v>
       </c>
       <c r="D25" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -4491,7 +5331,7 @@
         <v>Transformers Up</v>
       </c>
       <c r="D26" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -4503,7 +5343,7 @@
         <v>Grid-220V</v>
       </c>
       <c r="D27" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -4515,7 +5355,7 @@
         <v>Grid-400V</v>
       </c>
       <c r="D28" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -4527,7 +5367,7 @@
         <v>Grid-380V</v>
       </c>
       <c r="D29" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -4539,7 +5379,7 @@
         <v>Grid-225V</v>
       </c>
       <c r="D30" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -4551,7 +5391,7 @@
         <v>Grid-330V</v>
       </c>
       <c r="D31" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -4563,7 +5403,7 @@
         <v>Grid-275V</v>
       </c>
       <c r="D32" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -4575,7 +5415,7 @@
         <v>Grid-420V</v>
       </c>
       <c r="D33" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -4587,7 +5427,7 @@
         <v>Grid-300V</v>
       </c>
       <c r="D34" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -4599,7 +5439,7 @@
         <v>Grid-500V</v>
       </c>
       <c r="D35" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -4611,7 +5451,7 @@
         <v>Grid-750V</v>
       </c>
       <c r="D36" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -4623,7 +5463,7 @@
         <v>Grid-450V</v>
       </c>
       <c r="D37" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -4635,7 +5475,7 @@
         <v>Grid-515V</v>
       </c>
       <c r="D38" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -4647,7 +5487,7 @@
         <v>Grid-525V</v>
       </c>
       <c r="D39" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -4659,7 +5499,7 @@
         <v>Grid-320V</v>
       </c>
       <c r="D40" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -4671,7 +5511,7 @@
         <v>Grid-150V</v>
       </c>
       <c r="D41" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -4683,7 +5523,7 @@
         <v>Grid-270V</v>
       </c>
       <c r="D42" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -4695,7 +5535,7 @@
         <v>Grid-350V</v>
       </c>
       <c r="D43" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -4707,7 +5547,7 @@
         <v>Grid-250V</v>
       </c>
       <c r="D44" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -4719,7 +5559,7 @@
         <v>Grid-200V</v>
       </c>
       <c r="D45" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -4731,7 +5571,7 @@
         <v>Grid-236V</v>
       </c>
       <c r="D46" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -4743,7 +5583,7 @@
         <v>Grid-600V</v>
       </c>
       <c r="D47" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -4755,10 +5595,10 @@
         <v>Aggregators</v>
       </c>
       <c r="D48" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -4767,66 +5607,66 @@
         <v>DUMMY_IMP</v>
       </c>
       <c r="D49" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>70</v>
       </c>
+      <c r="B50" t="s">
+        <v>264</v>
+      </c>
       <c r="C50" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="E50" t="s">
-        <v>149</v>
-      </c>
-      <c r="F50" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>70</v>
       </c>
+      <c r="B51" t="s">
+        <v>264</v>
+      </c>
       <c r="C51" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="E51" t="s">
-        <v>150</v>
-      </c>
-      <c r="F51" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>70</v>
       </c>
       <c r="B52" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="C52" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="E52" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>70</v>
       </c>
       <c r="B53" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="C53" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E53" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -4837,7 +5677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -4848,7 +5688,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>70</v>
       </c>

</xml_diff>